<commit_message>
refactor: updated spreadsheet based on discussion
</commit_message>
<xml_diff>
--- a/docs/artifacts/rules/information-analytics-olav.xlsx
+++ b/docs/artifacts/rules/information-analytics-olav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\artifacts\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC32FD4-5CBA-44E2-9404-7333FD09974A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC2D15B-7C69-4090-A66B-16B69C1CBD0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41172" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="156">
   <si>
     <t>role</t>
   </si>
@@ -381,9 +381,6 @@
     <t>extended</t>
   </si>
   <si>
-    <t>power_analytics</t>
-  </si>
-  <si>
     <t>http://purl.org/cognite/power_analytic</t>
   </si>
   <si>
@@ -466,6 +463,36 @@
   </si>
   <si>
     <t>expectedPowerForecast</t>
+  </si>
+  <si>
+    <t>timeseriesForecast</t>
+  </si>
+  <si>
+    <t>power:GeneratingUnit</t>
+  </si>
+  <si>
+    <t>exact</t>
+  </si>
+  <si>
+    <t>power:GeoLocation</t>
+  </si>
+  <si>
+    <t>power: EnergyArea</t>
+  </si>
+  <si>
+    <t>power: windTurbines</t>
+  </si>
+  <si>
+    <t>analytics:WindTurbine</t>
+  </si>
+  <si>
+    <t>power:GenertingUnit</t>
+  </si>
+  <si>
+    <t>power:GenertingUnit[power:name]</t>
+  </si>
+  <si>
+    <t>analytics</t>
   </si>
 </sst>
 </file>
@@ -876,8 +903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -915,7 +942,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>118</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -923,7 +950,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -931,7 +958,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -939,7 +966,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -971,7 +998,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -984,11 +1011,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M47"/>
+  <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -997,7 +1024,9 @@
     <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="13" width="13" customWidth="1"/>
+    <col min="6" max="8" width="13" customWidth="1"/>
+    <col min="9" max="9" width="23.21875" customWidth="1"/>
+    <col min="10" max="13" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="25.8" x14ac:dyDescent="0.5">
@@ -1060,7 +1089,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>152</v>
       </c>
       <c r="B3" t="s">
         <v>30</v>
@@ -1074,10 +1103,16 @@
       <c r="G3">
         <v>1</v>
       </c>
+      <c r="I3" t="s">
+        <v>147</v>
+      </c>
+      <c r="J3" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>152</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
@@ -1091,10 +1126,16 @@
       <c r="G4">
         <v>1</v>
       </c>
+      <c r="I4" t="s">
+        <v>147</v>
+      </c>
+      <c r="J4" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>152</v>
       </c>
       <c r="B5" t="s">
         <v>33</v>
@@ -1108,10 +1149,16 @@
       <c r="G5">
         <v>1</v>
       </c>
+      <c r="I5" t="s">
+        <v>147</v>
+      </c>
+      <c r="J5" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>152</v>
       </c>
       <c r="B6" t="s">
         <v>35</v>
@@ -1125,10 +1172,16 @@
       <c r="G6">
         <v>1</v>
       </c>
+      <c r="I6" t="s">
+        <v>147</v>
+      </c>
+      <c r="J6" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>152</v>
       </c>
       <c r="B7" t="s">
         <v>38</v>
@@ -1142,10 +1195,16 @@
       <c r="G7">
         <v>1</v>
       </c>
+      <c r="I7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J7" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>152</v>
       </c>
       <c r="B8" t="s">
         <v>39</v>
@@ -1159,10 +1218,16 @@
       <c r="G8">
         <v>1</v>
       </c>
+      <c r="I8" t="s">
+        <v>55</v>
+      </c>
+      <c r="J8" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>152</v>
       </c>
       <c r="B9" t="s">
         <v>41</v>
@@ -1176,10 +1241,16 @@
       <c r="G9">
         <v>1</v>
       </c>
+      <c r="I9" t="s">
+        <v>55</v>
+      </c>
+      <c r="J9" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>152</v>
       </c>
       <c r="B10" t="s">
         <v>44</v>
@@ -1193,16 +1264,22 @@
       <c r="G10">
         <v>1</v>
       </c>
+      <c r="I10" t="s">
+        <v>55</v>
+      </c>
+      <c r="J10" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>152</v>
       </c>
       <c r="B11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1210,10 +1287,10 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>152</v>
       </c>
       <c r="B12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E12" t="s">
         <v>34</v>
@@ -1227,10 +1304,10 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>152</v>
       </c>
       <c r="B13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E13" t="s">
         <v>34</v>
@@ -1244,10 +1321,10 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>152</v>
       </c>
       <c r="B14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E14" t="s">
         <v>34</v>
@@ -1275,8 +1352,11 @@
       <c r="G16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I16" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -1292,8 +1372,11 @@
       <c r="G17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I17" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -1306,41 +1389,44 @@
       <c r="F18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I18" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>48</v>
       </c>
       <c r="B19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F19">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>48</v>
       </c>
       <c r="B20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>48</v>
       </c>
       <c r="B21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E21" t="s">
         <v>34</v>
@@ -1352,12 +1438,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>48</v>
       </c>
       <c r="B22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E22" t="s">
         <v>34</v>
@@ -1369,12 +1455,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E23" t="s">
         <v>34</v>
@@ -1386,9 +1472,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>85</v>
+        <v>122</v>
       </c>
       <c r="B25" t="s">
         <v>30</v>
@@ -1403,33 +1489,50 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>122</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>122</v>
+      </c>
+      <c r="B27" t="s">
+        <v>123</v>
+      </c>
+      <c r="E27" t="s">
+        <v>31</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>122</v>
+      </c>
+      <c r="B28" t="s">
+        <v>124</v>
+      </c>
+      <c r="E28" t="s">
         <v>86</v>
       </c>
-      <c r="B27" t="s">
-        <v>87</v>
-      </c>
-      <c r="E27" t="s">
-        <v>40</v>
-      </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-      <c r="G27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>86</v>
-      </c>
-      <c r="B28" t="s">
-        <v>88</v>
-      </c>
-      <c r="E28" t="s">
-        <v>40</v>
-      </c>
       <c r="F28">
         <v>1</v>
       </c>
@@ -1437,32 +1540,69 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>122</v>
+      </c>
+      <c r="B29" t="s">
+        <v>125</v>
+      </c>
+      <c r="E29" t="s">
+        <v>34</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>91</v>
+        <v>122</v>
       </c>
       <c r="B30" t="s">
-        <v>90</v>
+        <v>126</v>
       </c>
       <c r="E30" t="s">
-        <v>86</v>
+        <v>34</v>
       </c>
       <c r="F30">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>122</v>
+      </c>
+      <c r="B31" t="s">
+        <v>127</v>
+      </c>
+      <c r="E31" t="s">
+        <v>34</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
+        <v>128</v>
       </c>
       <c r="E32" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G32">
         <v>1</v>
@@ -1470,16 +1610,16 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>129</v>
       </c>
       <c r="E33" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G33">
         <v>1</v>
@@ -1487,50 +1627,33 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B34" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="E34" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>123</v>
-      </c>
-      <c r="B35" t="s">
-        <v>125</v>
-      </c>
-      <c r="E35" t="s">
-        <v>86</v>
-      </c>
-      <c r="F35">
-        <v>1</v>
-      </c>
-      <c r="G35">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="B36" t="s">
-        <v>126</v>
+        <v>30</v>
       </c>
       <c r="E36" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G36">
         <v>1</v>
@@ -1538,13 +1661,13 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="B37" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="E37" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -1555,10 +1678,10 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="B38" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="E38" t="s">
         <v>34</v>
@@ -1566,19 +1689,16 @@
       <c r="F38">
         <v>0</v>
       </c>
-      <c r="G38">
-        <v>1</v>
-      </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="B39" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="E39" t="s">
-        <v>34</v>
+        <v>138</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -1589,117 +1709,18 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="B40" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="E40" t="s">
         <v>34</v>
       </c>
       <c r="F40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>123</v>
-      </c>
-      <c r="B41" t="s">
-        <v>131</v>
-      </c>
-      <c r="E41" t="s">
-        <v>34</v>
-      </c>
-      <c r="F41">
-        <v>0</v>
-      </c>
-      <c r="G41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>134</v>
-      </c>
-      <c r="B43" t="s">
-        <v>30</v>
-      </c>
-      <c r="E43" t="s">
-        <v>31</v>
-      </c>
-      <c r="F43">
-        <v>1</v>
-      </c>
-      <c r="G43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>134</v>
-      </c>
-      <c r="B44" t="s">
-        <v>135</v>
-      </c>
-      <c r="E44" t="s">
-        <v>31</v>
-      </c>
-      <c r="F44">
-        <v>0</v>
-      </c>
-      <c r="G44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>134</v>
-      </c>
-      <c r="B45" t="s">
-        <v>136</v>
-      </c>
-      <c r="E45" t="s">
-        <v>34</v>
-      </c>
-      <c r="F45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>134</v>
-      </c>
-      <c r="B46" t="s">
-        <v>137</v>
-      </c>
-      <c r="E46" t="s">
-        <v>139</v>
-      </c>
-      <c r="F46">
-        <v>0</v>
-      </c>
-      <c r="G46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>134</v>
-      </c>
-      <c r="B47" t="s">
-        <v>138</v>
-      </c>
-      <c r="E47" t="s">
-        <v>34</v>
-      </c>
-      <c r="F47">
-        <v>1</v>
-      </c>
-      <c r="G47">
         <v>1</v>
       </c>
     </row>
@@ -1718,14 +1739,16 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.33203125" customWidth="1"/>
     <col min="2" max="2" width="17.88671875" customWidth="1"/>
-    <col min="3" max="7" width="13" customWidth="1"/>
+    <col min="3" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
@@ -1753,7 +1776,7 @@
         <v>16</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>22</v>
@@ -1776,6 +1799,12 @@
       <c r="A5" t="s">
         <v>85</v>
       </c>
+      <c r="E5" t="s">
+        <v>149</v>
+      </c>
+      <c r="F5" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -1784,6 +1813,12 @@
       <c r="B6" t="s">
         <v>85</v>
       </c>
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1792,15 +1827,21 @@
       <c r="B7" t="s">
         <v>85</v>
       </c>
+      <c r="E7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -1817,7 +1858,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A66" sqref="A3:G66"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1826,7 +1867,9 @@
     <col min="2" max="2" width="20.44140625" customWidth="1"/>
     <col min="3" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="24.44140625" customWidth="1"/>
-    <col min="6" max="13" width="13" customWidth="1"/>
+    <col min="6" max="8" width="13" customWidth="1"/>
+    <col min="9" max="9" width="31.33203125" customWidth="1"/>
+    <col min="10" max="13" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="25.8" x14ac:dyDescent="0.5">
@@ -1906,7 +1949,9 @@
         <v>1</v>
       </c>
       <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
+      <c r="I3" s="3" t="s">
+        <v>154</v>
+      </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -1931,7 +1976,9 @@
         <v>1</v>
       </c>
       <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
+      <c r="I4" s="3" t="s">
+        <v>153</v>
+      </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
@@ -1956,7 +2003,9 @@
         <v>1</v>
       </c>
       <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
+      <c r="I5" s="3" t="s">
+        <v>153</v>
+      </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
@@ -1981,7 +2030,9 @@
         <v>1</v>
       </c>
       <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+      <c r="I6" s="3" t="s">
+        <v>153</v>
+      </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
@@ -2021,7 +2072,9 @@
         <v>1</v>
       </c>
       <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+      <c r="I8" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
@@ -3324,8 +3377,8 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A28" sqref="A3:B28"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3553,7 +3606,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
[NEAT-145] Implementation analytic solution model (#354)
* docs: Download and set up metadata

* docs: Finished building the solution model as an information architect

* refactor; clean

* docs: Finish documentation

* refactor: fix

* refactor: review feedback

* docs; Remove work in progress warning

* refactor: updated spreadsheet based on discussion
</commit_message>
<xml_diff>
--- a/docs/artifacts/rules/information-analytics-olav.xlsx
+++ b/docs/artifacts/rules/information-analytics-olav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\artifacts\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75A2EE8-6DC0-4A4A-B033-9961421B6224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC2D15B-7C69-4090-A66B-16B69C1CBD0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41172" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="156">
   <si>
     <t>role</t>
   </si>
@@ -381,9 +381,6 @@
     <t>extended</t>
   </si>
   <si>
-    <t>power_analytics</t>
-  </si>
-  <si>
     <t>http://purl.org/cognite/power_analytic</t>
   </si>
   <si>
@@ -466,6 +463,36 @@
   </si>
   <si>
     <t>expectedPowerForecast</t>
+  </si>
+  <si>
+    <t>timeseriesForecast</t>
+  </si>
+  <si>
+    <t>power:GeneratingUnit</t>
+  </si>
+  <si>
+    <t>exact</t>
+  </si>
+  <si>
+    <t>power:GeoLocation</t>
+  </si>
+  <si>
+    <t>power: EnergyArea</t>
+  </si>
+  <si>
+    <t>power: windTurbines</t>
+  </si>
+  <si>
+    <t>analytics:WindTurbine</t>
+  </si>
+  <si>
+    <t>power:GenertingUnit</t>
+  </si>
+  <si>
+    <t>power:GenertingUnit[power:name]</t>
+  </si>
+  <si>
+    <t>analytics</t>
   </si>
 </sst>
 </file>
@@ -877,7 +904,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -906,13 +933,16 @@
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B3" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>118</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -920,7 +950,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -928,7 +958,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -936,7 +966,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -968,7 +998,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -981,11 +1011,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M47"/>
+  <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -994,7 +1024,9 @@
     <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="13" width="13" customWidth="1"/>
+    <col min="6" max="8" width="13" customWidth="1"/>
+    <col min="9" max="9" width="23.21875" customWidth="1"/>
+    <col min="10" max="13" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="25.8" x14ac:dyDescent="0.5">
@@ -1057,7 +1089,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>152</v>
       </c>
       <c r="B3" t="s">
         <v>30</v>
@@ -1071,10 +1103,16 @@
       <c r="G3">
         <v>1</v>
       </c>
+      <c r="I3" t="s">
+        <v>147</v>
+      </c>
+      <c r="J3" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>152</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
@@ -1088,10 +1126,16 @@
       <c r="G4">
         <v>1</v>
       </c>
+      <c r="I4" t="s">
+        <v>147</v>
+      </c>
+      <c r="J4" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>152</v>
       </c>
       <c r="B5" t="s">
         <v>33</v>
@@ -1105,10 +1149,16 @@
       <c r="G5">
         <v>1</v>
       </c>
+      <c r="I5" t="s">
+        <v>147</v>
+      </c>
+      <c r="J5" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>152</v>
       </c>
       <c r="B6" t="s">
         <v>35</v>
@@ -1122,10 +1172,16 @@
       <c r="G6">
         <v>1</v>
       </c>
+      <c r="I6" t="s">
+        <v>147</v>
+      </c>
+      <c r="J6" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>152</v>
       </c>
       <c r="B7" t="s">
         <v>38</v>
@@ -1139,10 +1195,16 @@
       <c r="G7">
         <v>1</v>
       </c>
+      <c r="I7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J7" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>152</v>
       </c>
       <c r="B8" t="s">
         <v>39</v>
@@ -1156,10 +1218,16 @@
       <c r="G8">
         <v>1</v>
       </c>
+      <c r="I8" t="s">
+        <v>55</v>
+      </c>
+      <c r="J8" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>152</v>
       </c>
       <c r="B9" t="s">
         <v>41</v>
@@ -1173,10 +1241,16 @@
       <c r="G9">
         <v>1</v>
       </c>
+      <c r="I9" t="s">
+        <v>55</v>
+      </c>
+      <c r="J9" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>152</v>
       </c>
       <c r="B10" t="s">
         <v>44</v>
@@ -1190,16 +1264,22 @@
       <c r="G10">
         <v>1</v>
       </c>
+      <c r="I10" t="s">
+        <v>55</v>
+      </c>
+      <c r="J10" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>152</v>
       </c>
       <c r="B11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1207,10 +1287,10 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>152</v>
       </c>
       <c r="B12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E12" t="s">
         <v>34</v>
@@ -1224,10 +1304,10 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>152</v>
       </c>
       <c r="B13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E13" t="s">
         <v>34</v>
@@ -1241,10 +1321,10 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>152</v>
       </c>
       <c r="B14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E14" t="s">
         <v>34</v>
@@ -1272,8 +1352,11 @@
       <c r="G16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I16" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -1289,8 +1372,11 @@
       <c r="G17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I17" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -1303,41 +1389,44 @@
       <c r="F18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I18" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>48</v>
       </c>
       <c r="B19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F19">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>48</v>
       </c>
       <c r="B20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>48</v>
       </c>
       <c r="B21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E21" t="s">
         <v>34</v>
@@ -1349,12 +1438,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>48</v>
       </c>
       <c r="B22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E22" t="s">
         <v>34</v>
@@ -1366,12 +1455,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E23" t="s">
         <v>34</v>
@@ -1383,9 +1472,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>85</v>
+        <v>122</v>
       </c>
       <c r="B25" t="s">
         <v>30</v>
@@ -1400,33 +1489,50 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>122</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>122</v>
+      </c>
+      <c r="B27" t="s">
+        <v>123</v>
+      </c>
+      <c r="E27" t="s">
+        <v>31</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>122</v>
+      </c>
+      <c r="B28" t="s">
+        <v>124</v>
+      </c>
+      <c r="E28" t="s">
         <v>86</v>
       </c>
-      <c r="B27" t="s">
-        <v>87</v>
-      </c>
-      <c r="E27" t="s">
-        <v>40</v>
-      </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-      <c r="G27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>86</v>
-      </c>
-      <c r="B28" t="s">
-        <v>88</v>
-      </c>
-      <c r="E28" t="s">
-        <v>40</v>
-      </c>
       <c r="F28">
         <v>1</v>
       </c>
@@ -1434,32 +1540,69 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>122</v>
+      </c>
+      <c r="B29" t="s">
+        <v>125</v>
+      </c>
+      <c r="E29" t="s">
+        <v>34</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>91</v>
+        <v>122</v>
       </c>
       <c r="B30" t="s">
-        <v>90</v>
+        <v>126</v>
       </c>
       <c r="E30" t="s">
-        <v>86</v>
+        <v>34</v>
       </c>
       <c r="F30">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>122</v>
+      </c>
+      <c r="B31" t="s">
+        <v>127</v>
+      </c>
+      <c r="E31" t="s">
+        <v>34</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
+        <v>128</v>
       </c>
       <c r="E32" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G32">
         <v>1</v>
@@ -1467,16 +1610,16 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>129</v>
       </c>
       <c r="E33" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G33">
         <v>1</v>
@@ -1484,50 +1627,33 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B34" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="E34" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>123</v>
-      </c>
-      <c r="B35" t="s">
-        <v>125</v>
-      </c>
-      <c r="E35" t="s">
-        <v>86</v>
-      </c>
-      <c r="F35">
-        <v>1</v>
-      </c>
-      <c r="G35">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="B36" t="s">
-        <v>126</v>
+        <v>30</v>
       </c>
       <c r="E36" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G36">
         <v>1</v>
@@ -1535,13 +1661,13 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="B37" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="E37" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -1552,10 +1678,10 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="B38" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="E38" t="s">
         <v>34</v>
@@ -1563,19 +1689,16 @@
       <c r="F38">
         <v>0</v>
       </c>
-      <c r="G38">
-        <v>1</v>
-      </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="B39" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="E39" t="s">
-        <v>34</v>
+        <v>138</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -1586,117 +1709,18 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="B40" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="E40" t="s">
         <v>34</v>
       </c>
       <c r="F40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>123</v>
-      </c>
-      <c r="B41" t="s">
-        <v>131</v>
-      </c>
-      <c r="E41" t="s">
-        <v>34</v>
-      </c>
-      <c r="F41">
-        <v>0</v>
-      </c>
-      <c r="G41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>134</v>
-      </c>
-      <c r="B43" t="s">
-        <v>30</v>
-      </c>
-      <c r="E43" t="s">
-        <v>31</v>
-      </c>
-      <c r="F43">
-        <v>1</v>
-      </c>
-      <c r="G43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>134</v>
-      </c>
-      <c r="B44" t="s">
-        <v>135</v>
-      </c>
-      <c r="E44" t="s">
-        <v>31</v>
-      </c>
-      <c r="F44">
-        <v>0</v>
-      </c>
-      <c r="G44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>134</v>
-      </c>
-      <c r="B45" t="s">
-        <v>136</v>
-      </c>
-      <c r="E45" t="s">
-        <v>34</v>
-      </c>
-      <c r="F45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>134</v>
-      </c>
-      <c r="B46" t="s">
-        <v>137</v>
-      </c>
-      <c r="E46" t="s">
-        <v>139</v>
-      </c>
-      <c r="F46">
-        <v>0</v>
-      </c>
-      <c r="G46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>134</v>
-      </c>
-      <c r="B47" t="s">
-        <v>138</v>
-      </c>
-      <c r="E47" t="s">
-        <v>34</v>
-      </c>
-      <c r="F47">
-        <v>1</v>
-      </c>
-      <c r="G47">
         <v>1</v>
       </c>
     </row>
@@ -1713,16 +1737,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.33203125" customWidth="1"/>
     <col min="2" max="2" width="17.88671875" customWidth="1"/>
-    <col min="3" max="7" width="13" customWidth="1"/>
+    <col min="3" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
@@ -1750,7 +1776,7 @@
         <v>16</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>22</v>
@@ -1773,6 +1799,12 @@
       <c r="A5" t="s">
         <v>85</v>
       </c>
+      <c r="E5" t="s">
+        <v>149</v>
+      </c>
+      <c r="F5" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -1781,6 +1813,12 @@
       <c r="B6" t="s">
         <v>85</v>
       </c>
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1789,15 +1827,21 @@
       <c r="B7" t="s">
         <v>85</v>
       </c>
+      <c r="E7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -1814,7 +1858,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A66" sqref="A3:G66"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1823,7 +1867,9 @@
     <col min="2" max="2" width="20.44140625" customWidth="1"/>
     <col min="3" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="24.44140625" customWidth="1"/>
-    <col min="6" max="13" width="13" customWidth="1"/>
+    <col min="6" max="8" width="13" customWidth="1"/>
+    <col min="9" max="9" width="31.33203125" customWidth="1"/>
+    <col min="10" max="13" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="25.8" x14ac:dyDescent="0.5">
@@ -1903,7 +1949,9 @@
         <v>1</v>
       </c>
       <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
+      <c r="I3" s="3" t="s">
+        <v>154</v>
+      </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -1928,7 +1976,9 @@
         <v>1</v>
       </c>
       <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
+      <c r="I4" s="3" t="s">
+        <v>153</v>
+      </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
@@ -1953,7 +2003,9 @@
         <v>1</v>
       </c>
       <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
+      <c r="I5" s="3" t="s">
+        <v>153</v>
+      </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
@@ -1978,7 +2030,9 @@
         <v>1</v>
       </c>
       <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+      <c r="I6" s="3" t="s">
+        <v>153</v>
+      </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
@@ -2018,7 +2072,9 @@
         <v>1</v>
       </c>
       <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+      <c r="I8" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
@@ -3321,8 +3377,8 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A28" sqref="A3:B28"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3550,7 +3606,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Neat 138 extend excel importer (#355)
First pass with ExcelImporter added which now handles reference and user Rules.
</commit_message>
<xml_diff>
--- a/docs/artifacts/rules/information-analytics-olav.xlsx
+++ b/docs/artifacts/rules/information-analytics-olav.xlsx
@@ -1,31 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\artifacts\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niva/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC2D15B-7C69-4090-A66B-16B69C1CBD0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F42E77-90FA-834B-AC54-BDD39E93BEAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
     <sheet name="Properties" sheetId="2" r:id="rId2"/>
     <sheet name="Classes" sheetId="3" r:id="rId3"/>
-    <sheet name="RefProperties" sheetId="4" r:id="rId4"/>
-    <sheet name="RefClasses" sheetId="5" r:id="rId5"/>
-    <sheet name="RefMetadata" sheetId="6" r:id="rId6"/>
+    <sheet name="ReferenceProperties" sheetId="4" r:id="rId4"/>
+    <sheet name="ReferenceClasses" sheetId="5" r:id="rId5"/>
+    <sheet name="ReferenceMetadata" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="147">
   <si>
     <t>role</t>
   </si>
@@ -381,6 +381,9 @@
     <t>extended</t>
   </si>
   <si>
+    <t>power_analytics</t>
+  </si>
+  <si>
     <t>http://purl.org/cognite/power_analytic</t>
   </si>
   <si>
@@ -463,36 +466,6 @@
   </si>
   <si>
     <t>expectedPowerForecast</t>
-  </si>
-  <si>
-    <t>timeseriesForecast</t>
-  </si>
-  <si>
-    <t>power:GeneratingUnit</t>
-  </si>
-  <si>
-    <t>exact</t>
-  </si>
-  <si>
-    <t>power:GeoLocation</t>
-  </si>
-  <si>
-    <t>power: EnergyArea</t>
-  </si>
-  <si>
-    <t>power: windTurbines</t>
-  </si>
-  <si>
-    <t>analytics:WindTurbine</t>
-  </si>
-  <si>
-    <t>power:GenertingUnit</t>
-  </si>
-  <si>
-    <t>power:GenertingUnit[power:name]</t>
-  </si>
-  <si>
-    <t>analytics</t>
   </si>
 </sst>
 </file>
@@ -502,7 +475,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -904,16 +877,16 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="48.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -921,7 +894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="16">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -929,47 +902,44 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="16">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:2" ht="16">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="16">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="16">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="16">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="16">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -977,7 +947,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="16">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -985,7 +955,7 @@
         <v>45377</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="16">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -993,12 +963,12 @@
         <v>45331</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="16">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1011,25 +981,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M40"/>
+  <dimension ref="A1:M47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K14" sqref="K14"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A32" sqref="A32:B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" customWidth="1"/>
+    <col min="1" max="1" width="34.5" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="23.21875" customWidth="1"/>
-    <col min="10" max="13" width="13" customWidth="1"/>
+    <col min="5" max="5" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="13" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:13" ht="26">
       <c r="A1" s="8" t="s">
         <v>12</v>
       </c>
@@ -1046,7 +1014,7 @@
       <c r="L1" s="9"/>
       <c r="M1" s="9"/>
     </row>
-    <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="19">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -1087,9 +1055,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>152</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
         <v>30</v>
@@ -1103,16 +1071,10 @@
       <c r="G3">
         <v>1</v>
       </c>
-      <c r="I3" t="s">
-        <v>147</v>
-      </c>
-      <c r="J3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>152</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
@@ -1126,16 +1088,10 @@
       <c r="G4">
         <v>1</v>
       </c>
-      <c r="I4" t="s">
-        <v>147</v>
-      </c>
-      <c r="J4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>152</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
         <v>33</v>
@@ -1149,16 +1105,10 @@
       <c r="G5">
         <v>1</v>
       </c>
-      <c r="I5" t="s">
-        <v>147</v>
-      </c>
-      <c r="J5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>152</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
         <v>35</v>
@@ -1172,16 +1122,10 @@
       <c r="G6">
         <v>1</v>
       </c>
-      <c r="I6" t="s">
-        <v>147</v>
-      </c>
-      <c r="J6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>152</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
         <v>38</v>
@@ -1195,16 +1139,10 @@
       <c r="G7">
         <v>1</v>
       </c>
-      <c r="I7" t="s">
-        <v>55</v>
-      </c>
-      <c r="J7" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>152</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
         <v>39</v>
@@ -1218,16 +1156,10 @@
       <c r="G8">
         <v>1</v>
       </c>
-      <c r="I8" t="s">
-        <v>55</v>
-      </c>
-      <c r="J8" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>152</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
         <v>41</v>
@@ -1241,16 +1173,10 @@
       <c r="G9">
         <v>1</v>
       </c>
-      <c r="I9" t="s">
-        <v>55</v>
-      </c>
-      <c r="J9" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
-        <v>152</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
         <v>44</v>
@@ -1264,33 +1190,27 @@
       <c r="G10">
         <v>1</v>
       </c>
-      <c r="I10" t="s">
-        <v>55</v>
-      </c>
-      <c r="J10" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>152</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E11" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>152</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E12" t="s">
         <v>34</v>
@@ -1302,12 +1222,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>152</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E13" t="s">
         <v>34</v>
@@ -1319,12 +1239,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>152</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E14" t="s">
         <v>34</v>
@@ -1336,7 +1256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -1352,11 +1272,8 @@
       <c r="G16">
         <v>1</v>
       </c>
-      <c r="I16" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -1372,11 +1289,8 @@
       <c r="G17">
         <v>1</v>
       </c>
-      <c r="I17" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -1389,44 +1303,41 @@
       <c r="F18">
         <v>0</v>
       </c>
-      <c r="I18" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>48</v>
       </c>
       <c r="B19" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E19" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F19">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>48</v>
       </c>
       <c r="B20" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E20" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>48</v>
       </c>
       <c r="B21" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E21" t="s">
         <v>34</v>
@@ -1438,12 +1349,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>48</v>
       </c>
       <c r="B22" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E22" t="s">
         <v>34</v>
@@ -1455,12 +1366,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E23" t="s">
         <v>34</v>
@@ -1472,9 +1383,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>122</v>
+        <v>85</v>
       </c>
       <c r="B25" t="s">
         <v>30</v>
@@ -1489,199 +1400,162 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>122</v>
-      </c>
-      <c r="B26" t="s">
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
+        <v>86</v>
+      </c>
+      <c r="B27" t="s">
+        <v>87</v>
+      </c>
+      <c r="E27" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
+        <v>86</v>
+      </c>
+      <c r="B28" t="s">
+        <v>88</v>
+      </c>
+      <c r="E28" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30" t="s">
+        <v>90</v>
+      </c>
+      <c r="E30" t="s">
+        <v>86</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
+        <v>123</v>
+      </c>
+      <c r="B32" t="s">
+        <v>30</v>
+      </c>
+      <c r="E32" t="s">
+        <v>31</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" t="s">
+        <v>123</v>
+      </c>
+      <c r="B33" t="s">
         <v>32</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E33" t="s">
         <v>31</v>
       </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-      <c r="G26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>122</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" t="s">
         <v>123</v>
       </c>
-      <c r="E27" t="s">
+      <c r="B34" t="s">
+        <v>124</v>
+      </c>
+      <c r="E34" t="s">
         <v>31</v>
       </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-      <c r="G27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>122</v>
-      </c>
-      <c r="B28" t="s">
-        <v>124</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" t="s">
+        <v>123</v>
+      </c>
+      <c r="B35" t="s">
+        <v>125</v>
+      </c>
+      <c r="E35" t="s">
         <v>86</v>
       </c>
-      <c r="F28">
-        <v>1</v>
-      </c>
-      <c r="G28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>122</v>
-      </c>
-      <c r="B29" t="s">
-        <v>125</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" t="s">
+        <v>123</v>
+      </c>
+      <c r="B36" t="s">
+        <v>126</v>
+      </c>
+      <c r="E36" t="s">
         <v>34</v>
       </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>122</v>
-      </c>
-      <c r="B30" t="s">
-        <v>126</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" t="s">
+        <v>123</v>
+      </c>
+      <c r="B37" t="s">
+        <v>127</v>
+      </c>
+      <c r="E37" t="s">
         <v>34</v>
       </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-      <c r="G30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>122</v>
-      </c>
-      <c r="B31" t="s">
-        <v>127</v>
-      </c>
-      <c r="E31" t="s">
-        <v>34</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-      <c r="G31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>122</v>
-      </c>
-      <c r="B32" t="s">
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" t="s">
+        <v>123</v>
+      </c>
+      <c r="B38" t="s">
         <v>128</v>
-      </c>
-      <c r="E32" t="s">
-        <v>34</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-      <c r="G32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>122</v>
-      </c>
-      <c r="B33" t="s">
-        <v>129</v>
-      </c>
-      <c r="E33" t="s">
-        <v>34</v>
-      </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
-      <c r="G33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>122</v>
-      </c>
-      <c r="B34" t="s">
-        <v>130</v>
-      </c>
-      <c r="E34" t="s">
-        <v>34</v>
-      </c>
-      <c r="F34">
-        <v>0</v>
-      </c>
-      <c r="G34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>146</v>
-      </c>
-      <c r="B36" t="s">
-        <v>30</v>
-      </c>
-      <c r="E36" t="s">
-        <v>31</v>
-      </c>
-      <c r="F36">
-        <v>1</v>
-      </c>
-      <c r="G36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>146</v>
-      </c>
-      <c r="B37" t="s">
-        <v>134</v>
-      </c>
-      <c r="E37" t="s">
-        <v>31</v>
-      </c>
-      <c r="F37">
-        <v>0</v>
-      </c>
-      <c r="G37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>146</v>
-      </c>
-      <c r="B38" t="s">
-        <v>135</v>
       </c>
       <c r="E38" t="s">
         <v>34</v>
@@ -1689,16 +1563,19 @@
       <c r="F38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>146</v>
+        <v>123</v>
       </c>
       <c r="B39" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E39" t="s">
-        <v>138</v>
+        <v>34</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -1707,20 +1584,119 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>146</v>
+        <v>123</v>
       </c>
       <c r="B40" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E40" t="s">
         <v>34</v>
       </c>
       <c r="F40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" t="s">
+        <v>123</v>
+      </c>
+      <c r="B41" t="s">
+        <v>131</v>
+      </c>
+      <c r="E41" t="s">
+        <v>34</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" t="s">
+        <v>134</v>
+      </c>
+      <c r="B43" t="s">
+        <v>30</v>
+      </c>
+      <c r="E43" t="s">
+        <v>31</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" t="s">
+        <v>134</v>
+      </c>
+      <c r="B44" t="s">
+        <v>135</v>
+      </c>
+      <c r="E44" t="s">
+        <v>31</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" t="s">
+        <v>134</v>
+      </c>
+      <c r="B45" t="s">
+        <v>136</v>
+      </c>
+      <c r="E45" t="s">
+        <v>34</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" t="s">
+        <v>134</v>
+      </c>
+      <c r="B46" t="s">
+        <v>137</v>
+      </c>
+      <c r="E46" t="s">
+        <v>139</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" t="s">
+        <v>134</v>
+      </c>
+      <c r="B47" t="s">
+        <v>138</v>
+      </c>
+      <c r="E47" t="s">
+        <v>34</v>
+      </c>
+      <c r="F47">
+        <v>1</v>
+      </c>
+      <c r="G47">
         <v>1</v>
       </c>
     </row>
@@ -1739,19 +1715,17 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="A3:B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" customWidth="1"/>
-    <col min="3" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" customWidth="1"/>
+    <col min="3" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" ht="26">
       <c r="A1" s="8" t="s">
         <v>26</v>
       </c>
@@ -1762,7 +1736,7 @@
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
     </row>
-    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="19">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -1776,7 +1750,7 @@
         <v>16</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>22</v>
@@ -1785,63 +1759,45 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>85</v>
       </c>
-      <c r="E5" t="s">
-        <v>149</v>
-      </c>
-      <c r="F5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>86</v>
       </c>
       <c r="B6" t="s">
         <v>85</v>
       </c>
-      <c r="E6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>91</v>
       </c>
       <c r="B7" t="s">
         <v>85</v>
       </c>
-      <c r="E7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1858,21 +1814,19 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:I12"/>
+      <selection pane="bottomLeft" activeCell="A66" sqref="A3:G66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" customWidth="1"/>
-    <col min="2" max="2" width="20.44140625" customWidth="1"/>
+    <col min="1" max="1" width="34.5" customWidth="1"/>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
     <col min="3" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="24.44140625" customWidth="1"/>
-    <col min="6" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="31.33203125" customWidth="1"/>
-    <col min="10" max="13" width="13" customWidth="1"/>
+    <col min="5" max="5" width="24.5" customWidth="1"/>
+    <col min="6" max="13" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:13" ht="26">
       <c r="A1" s="8" t="s">
         <v>12</v>
       </c>
@@ -1889,7 +1843,7 @@
       <c r="L1" s="9"/>
       <c r="M1" s="9"/>
     </row>
-    <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="19">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -1930,7 +1884,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13">
       <c r="A3" s="3" t="s">
         <v>29</v>
       </c>
@@ -1949,15 +1903,13 @@
         <v>1</v>
       </c>
       <c r="H3" s="3"/>
-      <c r="I3" s="3" t="s">
-        <v>154</v>
-      </c>
+      <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13">
       <c r="A4" s="3" t="s">
         <v>29</v>
       </c>
@@ -1976,15 +1928,13 @@
         <v>1</v>
       </c>
       <c r="H4" s="3"/>
-      <c r="I4" s="3" t="s">
-        <v>153</v>
-      </c>
+      <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13">
       <c r="A5" s="3" t="s">
         <v>29</v>
       </c>
@@ -2003,15 +1953,13 @@
         <v>1</v>
       </c>
       <c r="H5" s="3"/>
-      <c r="I5" s="3" t="s">
-        <v>153</v>
-      </c>
+      <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13">
       <c r="A6" s="3" t="s">
         <v>29</v>
       </c>
@@ -2030,15 +1978,13 @@
         <v>1</v>
       </c>
       <c r="H6" s="3"/>
-      <c r="I6" s="3" t="s">
-        <v>153</v>
-      </c>
+      <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -2053,7 +1999,7 @@
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13">
       <c r="A8" s="4" t="s">
         <v>37</v>
       </c>
@@ -2072,15 +2018,13 @@
         <v>1</v>
       </c>
       <c r="H8" s="4"/>
-      <c r="I8" s="4" t="s">
-        <v>55</v>
-      </c>
+      <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13">
       <c r="A9" s="4" t="s">
         <v>37</v>
       </c>
@@ -2105,7 +2049,7 @@
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13">
       <c r="A10" s="4" t="s">
         <v>37</v>
       </c>
@@ -2130,7 +2074,7 @@
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13">
       <c r="A11" s="4" t="s">
         <v>37</v>
       </c>
@@ -2155,7 +2099,7 @@
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13">
       <c r="A12" s="4" t="s">
         <v>37</v>
       </c>
@@ -2180,7 +2124,7 @@
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -2195,7 +2139,7 @@
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13">
       <c r="A14" s="3" t="s">
         <v>46</v>
       </c>
@@ -2220,7 +2164,7 @@
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13">
       <c r="A15" s="3" t="s">
         <v>46</v>
       </c>
@@ -2245,7 +2189,7 @@
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13">
       <c r="A16" s="3" t="s">
         <v>46</v>
       </c>
@@ -2270,7 +2214,7 @@
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13">
       <c r="A17" s="3" t="s">
         <v>46</v>
       </c>
@@ -2295,7 +2239,7 @@
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -2310,7 +2254,7 @@
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13">
       <c r="A19" s="4" t="s">
         <v>48</v>
       </c>
@@ -2335,7 +2279,7 @@
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13">
       <c r="A20" s="4" t="s">
         <v>48</v>
       </c>
@@ -2360,7 +2304,7 @@
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13">
       <c r="A21" s="4" t="s">
         <v>48</v>
       </c>
@@ -2383,7 +2327,7 @@
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13">
       <c r="A22" s="4" t="s">
         <v>48</v>
       </c>
@@ -2406,7 +2350,7 @@
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -2421,7 +2365,7 @@
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13">
       <c r="A24" s="3" t="s">
         <v>56</v>
       </c>
@@ -2446,7 +2390,7 @@
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13">
       <c r="A25" s="3" t="s">
         <v>56</v>
       </c>
@@ -2471,7 +2415,7 @@
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13">
       <c r="A26" s="3" t="s">
         <v>56</v>
       </c>
@@ -2496,7 +2440,7 @@
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13">
       <c r="A27" s="3" t="s">
         <v>56</v>
       </c>
@@ -2521,7 +2465,7 @@
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13">
       <c r="A28" s="3" t="s">
         <v>56</v>
       </c>
@@ -2546,7 +2490,7 @@
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13">
       <c r="A29" s="3" t="s">
         <v>56</v>
       </c>
@@ -2571,7 +2515,7 @@
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13">
       <c r="A30" s="3" t="s">
         <v>56</v>
       </c>
@@ -2596,7 +2540,7 @@
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13">
       <c r="A31" s="3" t="s">
         <v>56</v>
       </c>
@@ -2619,7 +2563,7 @@
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13">
       <c r="A32" s="3" t="s">
         <v>56</v>
       </c>
@@ -2642,7 +2586,7 @@
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13">
       <c r="A33" s="3" t="s">
         <v>56</v>
       </c>
@@ -2665,7 +2609,7 @@
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -2680,7 +2624,7 @@
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13">
       <c r="A35" s="4" t="s">
         <v>71</v>
       </c>
@@ -2705,7 +2649,7 @@
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13">
       <c r="A36" s="4" t="s">
         <v>71</v>
       </c>
@@ -2730,7 +2674,7 @@
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13">
       <c r="A37" s="4" t="s">
         <v>71</v>
       </c>
@@ -2755,7 +2699,7 @@
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13">
       <c r="A38" s="4" t="s">
         <v>71</v>
       </c>
@@ -2780,7 +2724,7 @@
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -2795,7 +2739,7 @@
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13">
       <c r="A40" s="3" t="s">
         <v>77</v>
       </c>
@@ -2820,7 +2764,7 @@
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13">
       <c r="A41" s="3" t="s">
         <v>77</v>
       </c>
@@ -2845,7 +2789,7 @@
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13">
       <c r="A42" s="3" t="s">
         <v>77</v>
       </c>
@@ -2868,7 +2812,7 @@
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -2883,7 +2827,7 @@
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13">
       <c r="A44" s="4" t="s">
         <v>83</v>
       </c>
@@ -2908,7 +2852,7 @@
       <c r="L44" s="4"/>
       <c r="M44" s="4"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13">
       <c r="A45" s="4" t="s">
         <v>83</v>
       </c>
@@ -2933,7 +2877,7 @@
       <c r="L45" s="4"/>
       <c r="M45" s="4"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13">
       <c r="A46" s="4" t="s">
         <v>83</v>
       </c>
@@ -2958,7 +2902,7 @@
       <c r="L46" s="4"/>
       <c r="M46" s="4"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -2973,7 +2917,7 @@
       <c r="L47" s="4"/>
       <c r="M47" s="4"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13">
       <c r="A48" s="3" t="s">
         <v>85</v>
       </c>
@@ -2998,7 +2942,7 @@
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -3013,7 +2957,7 @@
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13">
       <c r="A50" s="4" t="s">
         <v>86</v>
       </c>
@@ -3038,7 +2982,7 @@
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13">
       <c r="A51" s="4" t="s">
         <v>86</v>
       </c>
@@ -3063,7 +3007,7 @@
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -3078,7 +3022,7 @@
       <c r="L52" s="4"/>
       <c r="M52" s="4"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13">
       <c r="A53" s="3" t="s">
         <v>89</v>
       </c>
@@ -3101,7 +3045,7 @@
       <c r="L53" s="3"/>
       <c r="M53" s="3"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -3116,7 +3060,7 @@
       <c r="L54" s="3"/>
       <c r="M54" s="3"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13">
       <c r="A55" s="4" t="s">
         <v>91</v>
       </c>
@@ -3139,7 +3083,7 @@
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -3154,7 +3098,7 @@
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13">
       <c r="A57" s="3" t="s">
         <v>92</v>
       </c>
@@ -3179,7 +3123,7 @@
       <c r="L57" s="3"/>
       <c r="M57" s="3"/>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -3194,7 +3138,7 @@
       <c r="L58" s="3"/>
       <c r="M58" s="3"/>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13">
       <c r="A59" s="4" t="s">
         <v>94</v>
       </c>
@@ -3219,7 +3163,7 @@
       <c r="L59" s="4"/>
       <c r="M59" s="4"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -3234,7 +3178,7 @@
       <c r="L60" s="4"/>
       <c r="M60" s="4"/>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13">
       <c r="A61" s="3" t="s">
         <v>95</v>
       </c>
@@ -3259,7 +3203,7 @@
       <c r="L61" s="3"/>
       <c r="M61" s="3"/>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -3274,7 +3218,7 @@
       <c r="L62" s="3"/>
       <c r="M62" s="3"/>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13">
       <c r="A63" s="4" t="s">
         <v>96</v>
       </c>
@@ -3299,7 +3243,7 @@
       <c r="L63" s="4"/>
       <c r="M63" s="4"/>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
@@ -3314,7 +3258,7 @@
       <c r="L64" s="4"/>
       <c r="M64" s="4"/>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13">
       <c r="A65" s="3" t="s">
         <v>98</v>
       </c>
@@ -3339,7 +3283,7 @@
       <c r="L65" s="3"/>
       <c r="M65" s="3"/>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:13">
       <c r="A66" s="3" t="s">
         <v>98</v>
       </c>
@@ -3377,17 +3321,17 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
+      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A28" sqref="A3:B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="22.44140625" customWidth="1"/>
+    <col min="1" max="2" width="22.5" customWidth="1"/>
     <col min="3" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" ht="26">
       <c r="A1" s="8" t="s">
         <v>26</v>
       </c>
@@ -3398,7 +3342,7 @@
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
     </row>
-    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="19">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -3421,12 +3365,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -3434,12 +3378,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -3447,12 +3391,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>101</v>
       </c>
@@ -3460,7 +3404,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>102</v>
       </c>
@@ -3468,7 +3412,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>103</v>
       </c>
@@ -3476,7 +3420,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>104</v>
       </c>
@@ -3484,12 +3428,12 @@
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>105</v>
       </c>
@@ -3497,7 +3441,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>106</v>
       </c>
@@ -3505,7 +3449,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>107</v>
       </c>
@@ -3513,7 +3457,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>108</v>
       </c>
@@ -3521,17 +3465,17 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>109</v>
       </c>
@@ -3539,12 +3483,12 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>86</v>
       </c>
@@ -3552,7 +3496,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>89</v>
       </c>
@@ -3560,7 +3504,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>91</v>
       </c>
@@ -3568,27 +3512,27 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>98</v>
       </c>
@@ -3605,17 +3549,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="29.44140625" customWidth="1"/>
+    <col min="2" max="2" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3623,7 +3567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="16">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -3631,7 +3575,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="16">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -3639,7 +3583,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="16">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -3647,7 +3591,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="16">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -3655,7 +3599,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="16">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -3663,12 +3607,12 @@
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="16">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="16">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -3676,7 +3620,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="16">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -3684,7 +3628,7 @@
         <v>45377.41672594368</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="16">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -3692,7 +3636,7 @@
         <v>45377.41672594368</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="16">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
created analysis module to bundle up various methods
</commit_message>
<xml_diff>
--- a/docs/artifacts/rules/information-analytics-olav.xlsx
+++ b/docs/artifacts/rules/information-analytics-olav.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niva/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Secondary/repos/neat/docs/artifacts/rules/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F42E77-90FA-834B-AC54-BDD39E93BEAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3667237-8C7D-C84B-85F2-AEAA068B8044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41920" yWindow="500" windowWidth="26880" windowHeight="28300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -984,8 +984,8 @@
   <dimension ref="A1:M47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A32" sqref="A32:B41"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1812,9 +1812,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A66" sqref="A3:G66"/>
+      <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3322,7 +3322,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A28" sqref="A3:B28"/>
+      <selection pane="bottomLeft" activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3549,7 +3549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
created analysis module to bundle up various methods (#359)
Moved set of methods that were in _analysis module to be class methods.
Renamed methods (usually dropped "to" and "get")

This is prep for adding methods to the analysis class that will analyze rules to detect modeling scenarion.
</commit_message>
<xml_diff>
--- a/docs/artifacts/rules/information-analytics-olav.xlsx
+++ b/docs/artifacts/rules/information-analytics-olav.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niva/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Secondary/repos/neat/docs/artifacts/rules/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F42E77-90FA-834B-AC54-BDD39E93BEAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3667237-8C7D-C84B-85F2-AEAA068B8044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41920" yWindow="500" windowWidth="26880" windowHeight="28300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -984,8 +984,8 @@
   <dimension ref="A1:M47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A32" sqref="A32:B41"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1812,9 +1812,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A66" sqref="A3:G66"/>
+      <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3322,7 +3322,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A28" sqref="A3:B28"/>
+      <selection pane="bottomLeft" activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3549,7 +3549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
moved from Referance<> top Ref<>
</commit_message>
<xml_diff>
--- a/docs/artifacts/rules/information-analytics-olav.xlsx
+++ b/docs/artifacts/rules/information-analytics-olav.xlsx
@@ -5,20 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niva/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Secondary/repos/neat/docs/artifacts/rules/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0357DA-7653-3946-B79F-0E57113CCAF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7179DD1F-DDFC-124D-80AF-6E33644A197D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
     <sheet name="Properties" sheetId="2" r:id="rId2"/>
     <sheet name="Classes" sheetId="3" r:id="rId3"/>
-    <sheet name="ReferenceProperties" sheetId="4" r:id="rId4"/>
-    <sheet name="ReferenceClasses" sheetId="5" r:id="rId5"/>
-    <sheet name="ReferenceMetadata" sheetId="6" r:id="rId6"/>
+    <sheet name="RefProperties" sheetId="4" r:id="rId4"/>
+    <sheet name="RefClasses" sheetId="5" r:id="rId5"/>
+    <sheet name="RefMetadata" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1841,7 +1841,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D55" sqref="D55"/>
     </sheetView>
@@ -1935,7 +1935,7 @@
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!A3 &amp; "(" &amp; ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!B3 &amp; ")"</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A3 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B3 &amp; ")"</f>
         <v>power:GeneratingUnit(power:name)</v>
       </c>
       <c r="J3" s="3"/>
@@ -1963,7 +1963,7 @@
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!A4 &amp; "(" &amp; ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!B4 &amp; ")"</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A4 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B4 &amp; ")"</f>
         <v>power:GeneratingUnit(power:type)</v>
       </c>
       <c r="J4" s="3"/>
@@ -1991,7 +1991,7 @@
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!A5 &amp; "(" &amp; ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!B5 &amp; ")"</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A5 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B5 &amp; ")"</f>
         <v>power:GeneratingUnit(power:activePower)</v>
       </c>
       <c r="J5" s="3"/>
@@ -2019,7 +2019,7 @@
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!A6 &amp; "(" &amp; ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!B6 &amp; ")"</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A6 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B6 &amp; ")"</f>
         <v>power:GeneratingUnit(power:geoLocation)</v>
       </c>
       <c r="J6" s="3"/>
@@ -2062,7 +2062,7 @@
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!A8 &amp; "(" &amp; ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!B8 &amp; ")"</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A8 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B8 &amp; ")"</f>
         <v>power:WindTurbine(power:manufacturer)</v>
       </c>
       <c r="J8" s="4"/>
@@ -2090,7 +2090,7 @@
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!A9 &amp; "(" &amp; ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!B9 &amp; ")"</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A9 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B9 &amp; ")"</f>
         <v>power:WindTurbine(power:ratedPower)</v>
       </c>
       <c r="J9" s="4"/>
@@ -2118,7 +2118,7 @@
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!A10 &amp; "(" &amp; ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!B10 &amp; ")"</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A10 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B10 &amp; ")"</f>
         <v>power:WindTurbine(power:hubHeight)</v>
       </c>
       <c r="J10" s="4"/>
@@ -2146,7 +2146,7 @@
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!A11 &amp; "(" &amp; ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!B11 &amp; ")"</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A11 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B11 &amp; ")"</f>
         <v>power:WindTurbine(power:arrayCableConnection)</v>
       </c>
       <c r="J11" s="4"/>
@@ -2174,7 +2174,7 @@
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!A12 &amp; "(" &amp; ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!B12 &amp; ")"</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A12 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B12 &amp; ")"</f>
         <v>power:WindTurbine(power:lifeExpectancy)</v>
       </c>
       <c r="J12" s="4"/>
@@ -2217,7 +2217,7 @@
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!A14 &amp; "(" &amp; ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!B14 &amp; ")"</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A14 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B14 &amp; ")"</f>
         <v>power:EnergyArea(power:name)</v>
       </c>
       <c r="J14" s="3"/>
@@ -2245,7 +2245,7 @@
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!A15 &amp; "(" &amp; ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!B15 &amp; ")"</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A15 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B15 &amp; ")"</f>
         <v>power:EnergyArea(power:geoLocation)</v>
       </c>
       <c r="J15" s="3"/>
@@ -2273,7 +2273,7 @@
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!A16 &amp; "(" &amp; ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!B16 &amp; ")"</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A16 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B16 &amp; ")"</f>
         <v>power:EnergyArea(power:ratedPower)</v>
       </c>
       <c r="J16" s="3"/>
@@ -2301,7 +2301,7 @@
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!A17 &amp; "(" &amp; ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!B17 &amp; ")"</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A17 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B17 &amp; ")"</f>
         <v>power:EnergyArea(power:activePower)</v>
       </c>
       <c r="J17" s="3"/>
@@ -2344,7 +2344,7 @@
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="4" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!A19 &amp; "(" &amp; ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!B19 &amp; ")"</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A19 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B19 &amp; ")"</f>
         <v>power:WindFarm(power:substation)</v>
       </c>
       <c r="J19" s="4"/>
@@ -2372,7 +2372,7 @@
       </c>
       <c r="H20" s="4"/>
       <c r="I20" s="4" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!A20 &amp; "(" &amp; ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!B20 &amp; ")"</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A20 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B20 &amp; ")"</f>
         <v>power:WindFarm(power:exportCable)</v>
       </c>
       <c r="J20" s="4"/>
@@ -2398,7 +2398,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!A21 &amp; "(" &amp; ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!B21 &amp; ")"</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A21 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B21 &amp; ")"</f>
         <v>power:WindFarm(power:arrayCable)</v>
       </c>
       <c r="J21" s="4"/>
@@ -2424,7 +2424,7 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!A22 &amp; "(" &amp; ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!B22 &amp; ")"</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A22 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B22 &amp; ")"</f>
         <v>power:WindFarm(power:windTurbines)</v>
       </c>
       <c r="J22" s="4"/>
@@ -2467,7 +2467,7 @@
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="3" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!A24 &amp; "(" &amp; ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!B24 &amp; ")"</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A24 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B24 &amp; ")"</f>
         <v>power:Substation(power:name)</v>
       </c>
       <c r="J24" s="3"/>
@@ -2495,7 +2495,7 @@
       </c>
       <c r="H25" s="3"/>
       <c r="I25" s="3" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!A25 &amp; "(" &amp; ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!B25 &amp; ")"</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A25 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B25 &amp; ")"</f>
         <v>power:Substation(power:location)</v>
       </c>
       <c r="J25" s="3"/>
@@ -2523,7 +2523,7 @@
       </c>
       <c r="H26" s="3"/>
       <c r="I26" s="3" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!A26 &amp; "(" &amp; ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!B26 &amp; ")"</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A26 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B26 &amp; ")"</f>
         <v>power:Substation(power:mainTransformer)</v>
       </c>
       <c r="J26" s="3"/>
@@ -2551,7 +2551,7 @@
       </c>
       <c r="H27" s="3"/>
       <c r="I27" s="3" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!A27 &amp; "(" &amp; ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!B27 &amp; ")"</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A27 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B27 &amp; ")"</f>
         <v>power:Substation(power:primaryPowerLine)</v>
       </c>
       <c r="J27" s="3"/>
@@ -2579,7 +2579,7 @@
       </c>
       <c r="H28" s="3"/>
       <c r="I28" s="3" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!A28 &amp; "(" &amp; ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!B28 &amp; ")"</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A28 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B28 &amp; ")"</f>
         <v>power:Substation(power:secondaryPowerLine)</v>
       </c>
       <c r="J28" s="3"/>
@@ -2607,7 +2607,7 @@
       </c>
       <c r="H29" s="3"/>
       <c r="I29" s="3" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!A29 &amp; "(" &amp; ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!B29 &amp; ")"</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A29 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B29 &amp; ")"</f>
         <v>power:Substation(power:primaryVoltage)</v>
       </c>
       <c r="J29" s="3"/>
@@ -2635,7 +2635,7 @@
       </c>
       <c r="H30" s="3"/>
       <c r="I30" s="3" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!A30 &amp; "(" &amp; ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!B30 &amp; ")"</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A30 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B30 &amp; ")"</f>
         <v>power:Substation(power:secondaryVoltage)</v>
       </c>
       <c r="J30" s="3"/>
@@ -2661,7 +2661,7 @@
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="3" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!A31 &amp; "(" &amp; ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!B31 &amp; ")"</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A31 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B31 &amp; ")"</f>
         <v>power:Substation(power:circuitBreaker)</v>
       </c>
       <c r="J31" s="3"/>
@@ -2687,7 +2687,7 @@
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
       <c r="I32" s="3" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!A32 &amp; "(" &amp; ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!B32 &amp; ")"</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A32 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B32 &amp; ")"</f>
         <v>power:Substation(power:disconnectSwitch)</v>
       </c>
       <c r="J32" s="3"/>
@@ -2713,7 +2713,7 @@
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="I33" s="3" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!A33 &amp; "(" &amp; ReferenceMetadata!B4&amp; ":" &amp;ReferenceProperties!B33 &amp; ")"</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A33 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B33 &amp; ")"</f>
         <v>power:Substation(power:currentTransformer)</v>
       </c>
       <c r="J33" s="3"/>
@@ -3485,7 +3485,7 @@
         <v>28</v>
       </c>
       <c r="E3" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceClasses!A3</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A3</f>
         <v>power:GeneratingUnit</v>
       </c>
     </row>
@@ -3497,7 +3497,7 @@
         <v>28</v>
       </c>
       <c r="E4" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceClasses!A4</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A4</f>
         <v>power:WindTurbine</v>
       </c>
     </row>
@@ -3506,7 +3506,7 @@
         <v>45</v>
       </c>
       <c r="E5" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceClasses!A5</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A5</f>
         <v>power:EnergyArea</v>
       </c>
     </row>
@@ -3518,7 +3518,7 @@
         <v>45</v>
       </c>
       <c r="E6" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceClasses!A6</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A6</f>
         <v>power:WindFarm</v>
       </c>
     </row>
@@ -3527,7 +3527,7 @@
         <v>55</v>
       </c>
       <c r="E7" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceClasses!A7</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A7</f>
         <v>power:Substation</v>
       </c>
     </row>
@@ -3539,7 +3539,7 @@
         <v>55</v>
       </c>
       <c r="E8" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceClasses!A8</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A8</f>
         <v>power:OffshoreSubstation</v>
       </c>
     </row>
@@ -3551,7 +3551,7 @@
         <v>55</v>
       </c>
       <c r="E9" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceClasses!A9</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A9</f>
         <v>power:TransmissionSubstation</v>
       </c>
     </row>
@@ -3563,7 +3563,7 @@
         <v>55</v>
       </c>
       <c r="E10" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceClasses!A10</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A10</f>
         <v>power:DistributionSubstation</v>
       </c>
     </row>
@@ -3575,7 +3575,7 @@
         <v>101</v>
       </c>
       <c r="E11" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceClasses!A11</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A11</f>
         <v>power:OnshoreSubstation</v>
       </c>
     </row>
@@ -3584,7 +3584,7 @@
         <v>70</v>
       </c>
       <c r="E12" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceClasses!A12</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A12</f>
         <v>power:PowerLine</v>
       </c>
     </row>
@@ -3596,7 +3596,7 @@
         <v>70</v>
       </c>
       <c r="E13" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceClasses!A13</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A13</f>
         <v>power:ArrayCable</v>
       </c>
     </row>
@@ -3608,7 +3608,7 @@
         <v>70</v>
       </c>
       <c r="E14" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceClasses!A14</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A14</f>
         <v>power:ExportCable</v>
       </c>
     </row>
@@ -3620,7 +3620,7 @@
         <v>70</v>
       </c>
       <c r="E15" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceClasses!A15</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A15</f>
         <v>power:Transmission</v>
       </c>
     </row>
@@ -3632,7 +3632,7 @@
         <v>70</v>
       </c>
       <c r="E16" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceClasses!A16</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A16</f>
         <v>power:DistributionLine</v>
       </c>
     </row>
@@ -3641,7 +3641,7 @@
         <v>76</v>
       </c>
       <c r="E17" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceClasses!A17</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A17</f>
         <v>power:Meter</v>
       </c>
     </row>
@@ -3650,7 +3650,7 @@
         <v>82</v>
       </c>
       <c r="E18" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceClasses!A18</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A18</f>
         <v>power:EnergyConsumer</v>
       </c>
     </row>
@@ -3662,7 +3662,7 @@
         <v>82</v>
       </c>
       <c r="E19" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceClasses!A19</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A19</f>
         <v>power:ElectricCarCharger</v>
       </c>
     </row>
@@ -3671,7 +3671,7 @@
         <v>84</v>
       </c>
       <c r="E20" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceClasses!A20</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A20</f>
         <v>power:GeoLocation</v>
       </c>
     </row>
@@ -3683,7 +3683,7 @@
         <v>84</v>
       </c>
       <c r="E21" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceClasses!A21</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A21</f>
         <v>power:Point</v>
       </c>
     </row>
@@ -3695,7 +3695,7 @@
         <v>84</v>
       </c>
       <c r="E22" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceClasses!A22</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A22</f>
         <v>power:MultiLineString</v>
       </c>
     </row>
@@ -3707,7 +3707,7 @@
         <v>84</v>
       </c>
       <c r="E23" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceClasses!A23</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A23</f>
         <v>power:Polygon</v>
       </c>
     </row>
@@ -3716,7 +3716,7 @@
         <v>91</v>
       </c>
       <c r="E24" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceClasses!A24</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A24</f>
         <v>power:CircuitBreaker</v>
       </c>
     </row>
@@ -3725,7 +3725,7 @@
         <v>93</v>
       </c>
       <c r="E25" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceClasses!A25</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A25</f>
         <v>power:CurrentTransformer</v>
       </c>
     </row>
@@ -3734,7 +3734,7 @@
         <v>94</v>
       </c>
       <c r="E26" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceClasses!A26</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A26</f>
         <v>power:DisconnectSwitch</v>
       </c>
     </row>
@@ -3743,7 +3743,7 @@
         <v>95</v>
       </c>
       <c r="E27" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceClasses!A27</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A27</f>
         <v>power:VoltageLevel</v>
       </c>
     </row>
@@ -3752,7 +3752,7 @@
         <v>97</v>
       </c>
       <c r="E28" t="str">
-        <f>ReferenceMetadata!B4&amp; ":" &amp;ReferenceClasses!A28</f>
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A28</f>
         <v>power:VoltageTransformer</v>
       </c>
     </row>
@@ -3768,7 +3768,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Neat 155 info detect modeling use case (#364)
Still in making
</commit_message>
<xml_diff>
--- a/docs/artifacts/rules/information-analytics-olav.xlsx
+++ b/docs/artifacts/rules/information-analytics-olav.xlsx
@@ -8,24 +8,36 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Secondary/repos/neat/docs/artifacts/rules/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3667237-8C7D-C84B-85F2-AEAA068B8044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7179DD1F-DDFC-124D-80AF-6E33644A197D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41920" yWindow="500" windowWidth="26880" windowHeight="28300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
     <sheet name="Properties" sheetId="2" r:id="rId2"/>
     <sheet name="Classes" sheetId="3" r:id="rId3"/>
-    <sheet name="ReferenceProperties" sheetId="4" r:id="rId4"/>
-    <sheet name="ReferenceClasses" sheetId="5" r:id="rId5"/>
-    <sheet name="ReferenceMetadata" sheetId="6" r:id="rId6"/>
+    <sheet name="RefProperties" sheetId="4" r:id="rId4"/>
+    <sheet name="RefClasses" sheetId="5" r:id="rId5"/>
+    <sheet name="RefMetadata" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="148">
   <si>
     <t>role</t>
   </si>
@@ -111,9 +123,6 @@
     <t>Parent Class</t>
   </si>
   <si>
-    <t>Source</t>
-  </si>
-  <si>
     <t>GeneratingUnit</t>
   </si>
   <si>
@@ -466,6 +475,12 @@
   </si>
   <si>
     <t>expectedPowerForecast</t>
+  </si>
+  <si>
+    <t>power:WindFarm</t>
+  </si>
+  <si>
+    <t>power:GeoLocation</t>
   </si>
 </sst>
 </file>
@@ -475,7 +490,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -487,16 +502,19 @@
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="20"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -877,16 +895,16 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="48.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16">
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -894,60 +912,60 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16">
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="16">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16">
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="16">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="16">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="16">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="16">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="16">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -955,7 +973,7 @@
         <v>45377</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="16">
+    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -963,12 +981,12 @@
         <v>45331</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="16">
+    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -984,11 +1002,11 @@
   <dimension ref="A1:M47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
+      <pane ySplit="2" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.5" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
@@ -997,7 +1015,7 @@
     <col min="6" max="13" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="26">
+    <row r="1" spans="1:13" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>12</v>
       </c>
@@ -1014,7 +1032,7 @@
       <c r="L1" s="9"/>
       <c r="M1" s="9"/>
     </row>
-    <row r="2" spans="1:13" ht="19">
+    <row r="2" spans="1:13" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -1055,643 +1073,643 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
         <v>37</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E7" t="s">
         <v>30</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" t="s">
+        <v>139</v>
+      </c>
+      <c r="E11" t="s">
+        <v>133</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>140</v>
+      </c>
+      <c r="E12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>141</v>
+      </c>
+      <c r="E13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>142</v>
+      </c>
+      <c r="E14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" t="s">
+        <v>90</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" t="s">
+        <v>131</v>
+      </c>
+      <c r="E19" t="s">
+        <v>122</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" t="s">
+        <v>132</v>
+      </c>
+      <c r="E20" t="s">
+        <v>122</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" t="s">
+        <v>143</v>
+      </c>
+      <c r="E21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" t="s">
+        <v>144</v>
+      </c>
+      <c r="E22" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" t="s">
+        <v>145</v>
+      </c>
+      <c r="E23" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>85</v>
+      </c>
+      <c r="B27" t="s">
+        <v>86</v>
+      </c>
+      <c r="E27" t="s">
+        <v>39</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" t="s">
+        <v>87</v>
+      </c>
+      <c r="E28" t="s">
+        <v>39</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" t="s">
+        <v>89</v>
+      </c>
+      <c r="E30" t="s">
+        <v>85</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>122</v>
+      </c>
+      <c r="B32" t="s">
+        <v>29</v>
+      </c>
+      <c r="E32" t="s">
+        <v>30</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>122</v>
+      </c>
+      <c r="B33" t="s">
         <v>31</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="E33" t="s">
+        <v>30</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>122</v>
+      </c>
+      <c r="B34" t="s">
+        <v>123</v>
+      </c>
+      <c r="E34" t="s">
+        <v>30</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>122</v>
+      </c>
+      <c r="B35" t="s">
+        <v>124</v>
+      </c>
+      <c r="E35" t="s">
+        <v>85</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>122</v>
+      </c>
+      <c r="B36" t="s">
+        <v>125</v>
+      </c>
+      <c r="E36" t="s">
         <v>33</v>
       </c>
-      <c r="E5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" t="s">
-        <v>140</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>122</v>
+      </c>
+      <c r="B37" t="s">
+        <v>126</v>
+      </c>
+      <c r="E37" t="s">
+        <v>33</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>122</v>
+      </c>
+      <c r="B38" t="s">
+        <v>127</v>
+      </c>
+      <c r="E38" t="s">
+        <v>33</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>122</v>
+      </c>
+      <c r="B39" t="s">
+        <v>128</v>
+      </c>
+      <c r="E39" t="s">
+        <v>33</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>122</v>
+      </c>
+      <c r="B40" t="s">
+        <v>129</v>
+      </c>
+      <c r="E40" t="s">
+        <v>33</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>122</v>
+      </c>
+      <c r="B41" t="s">
+        <v>130</v>
+      </c>
+      <c r="E41" t="s">
+        <v>33</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>133</v>
+      </c>
+      <c r="B43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E43" t="s">
+        <v>30</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>133</v>
+      </c>
+      <c r="B44" t="s">
         <v>134</v>
       </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" t="s">
-        <v>141</v>
-      </c>
-      <c r="E12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" t="s">
-        <v>142</v>
-      </c>
-      <c r="E13" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" t="s">
-        <v>143</v>
-      </c>
-      <c r="E14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="E44" t="s">
         <v>30</v>
       </c>
-      <c r="E16" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" t="s">
-        <v>91</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" t="s">
-        <v>54</v>
-      </c>
-      <c r="E18" t="s">
-        <v>37</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" t="s">
-        <v>132</v>
-      </c>
-      <c r="E19" t="s">
-        <v>123</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>133</v>
       </c>
-      <c r="E20" t="s">
-        <v>123</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" t="s">
-        <v>144</v>
-      </c>
-      <c r="E21" t="s">
-        <v>34</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" t="s">
-        <v>145</v>
-      </c>
-      <c r="E22" t="s">
-        <v>34</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" t="s">
-        <v>146</v>
-      </c>
-      <c r="E23" t="s">
-        <v>34</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" t="s">
-        <v>85</v>
-      </c>
-      <c r="B25" t="s">
-        <v>30</v>
-      </c>
-      <c r="E25" t="s">
-        <v>31</v>
-      </c>
-      <c r="F25">
-        <v>1</v>
-      </c>
-      <c r="G25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" t="s">
-        <v>86</v>
-      </c>
-      <c r="B27" t="s">
-        <v>87</v>
-      </c>
-      <c r="E27" t="s">
-        <v>40</v>
-      </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-      <c r="G27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" t="s">
-        <v>86</v>
-      </c>
-      <c r="B28" t="s">
-        <v>88</v>
-      </c>
-      <c r="E28" t="s">
-        <v>40</v>
-      </c>
-      <c r="F28">
-        <v>1</v>
-      </c>
-      <c r="G28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" t="s">
-        <v>91</v>
-      </c>
-      <c r="B30" t="s">
-        <v>90</v>
-      </c>
-      <c r="E30" t="s">
-        <v>86</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" t="s">
-        <v>123</v>
-      </c>
-      <c r="B32" t="s">
-        <v>30</v>
-      </c>
-      <c r="E32" t="s">
-        <v>31</v>
-      </c>
-      <c r="F32">
-        <v>1</v>
-      </c>
-      <c r="G32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" t="s">
-        <v>123</v>
-      </c>
-      <c r="B33" t="s">
-        <v>32</v>
-      </c>
-      <c r="E33" t="s">
-        <v>31</v>
-      </c>
-      <c r="F33">
-        <v>1</v>
-      </c>
-      <c r="G33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" t="s">
-        <v>123</v>
-      </c>
-      <c r="B34" t="s">
-        <v>124</v>
-      </c>
-      <c r="E34" t="s">
-        <v>31</v>
-      </c>
-      <c r="F34">
-        <v>1</v>
-      </c>
-      <c r="G34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" t="s">
-        <v>123</v>
-      </c>
-      <c r="B35" t="s">
-        <v>125</v>
-      </c>
-      <c r="E35" t="s">
-        <v>86</v>
-      </c>
-      <c r="F35">
-        <v>1</v>
-      </c>
-      <c r="G35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" t="s">
-        <v>123</v>
-      </c>
-      <c r="B36" t="s">
-        <v>126</v>
-      </c>
-      <c r="E36" t="s">
-        <v>34</v>
-      </c>
-      <c r="F36">
-        <v>0</v>
-      </c>
-      <c r="G36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="A37" t="s">
-        <v>123</v>
-      </c>
-      <c r="B37" t="s">
-        <v>127</v>
-      </c>
-      <c r="E37" t="s">
-        <v>34</v>
-      </c>
-      <c r="F37">
-        <v>0</v>
-      </c>
-      <c r="G37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38" t="s">
-        <v>123</v>
-      </c>
-      <c r="B38" t="s">
-        <v>128</v>
-      </c>
-      <c r="E38" t="s">
-        <v>34</v>
-      </c>
-      <c r="F38">
-        <v>0</v>
-      </c>
-      <c r="G38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="A39" t="s">
-        <v>123</v>
-      </c>
-      <c r="B39" t="s">
-        <v>129</v>
-      </c>
-      <c r="E39" t="s">
-        <v>34</v>
-      </c>
-      <c r="F39">
-        <v>0</v>
-      </c>
-      <c r="G39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40" t="s">
-        <v>123</v>
-      </c>
-      <c r="B40" t="s">
-        <v>130</v>
-      </c>
-      <c r="E40" t="s">
-        <v>34</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
-      <c r="G40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" t="s">
-        <v>123</v>
-      </c>
-      <c r="B41" t="s">
-        <v>131</v>
-      </c>
-      <c r="E41" t="s">
-        <v>34</v>
-      </c>
-      <c r="F41">
-        <v>0</v>
-      </c>
-      <c r="G41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43" t="s">
-        <v>134</v>
-      </c>
-      <c r="B43" t="s">
-        <v>30</v>
-      </c>
-      <c r="E43" t="s">
-        <v>31</v>
-      </c>
-      <c r="F43">
-        <v>1</v>
-      </c>
-      <c r="G43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="A44" t="s">
-        <v>134</v>
-      </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>135</v>
       </c>
-      <c r="E44" t="s">
-        <v>31</v>
-      </c>
-      <c r="F44">
-        <v>0</v>
-      </c>
-      <c r="G44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="A45" t="s">
-        <v>134</v>
-      </c>
-      <c r="B45" t="s">
+      <c r="E45" t="s">
+        <v>33</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>133</v>
+      </c>
+      <c r="B46" t="s">
         <v>136</v>
       </c>
-      <c r="E45" t="s">
-        <v>34</v>
-      </c>
-      <c r="F45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
-      <c r="A46" t="s">
-        <v>134</v>
-      </c>
-      <c r="B46" t="s">
+      <c r="E46" t="s">
+        <v>138</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>133</v>
+      </c>
+      <c r="B47" t="s">
         <v>137</v>
       </c>
-      <c r="E46" t="s">
-        <v>139</v>
-      </c>
-      <c r="F46">
-        <v>0</v>
-      </c>
-      <c r="G46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47" t="s">
-        <v>134</v>
-      </c>
-      <c r="B47" t="s">
-        <v>138</v>
-      </c>
       <c r="E47" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F47">
         <v>1</v>
@@ -1715,17 +1733,19 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="A3:B13"/>
+      <selection pane="bottomLeft" activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.33203125" customWidth="1"/>
     <col min="2" max="2" width="17.83203125" customWidth="1"/>
-    <col min="3" max="7" width="13" customWidth="1"/>
+    <col min="3" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26">
+    <row r="1" spans="1:7" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>26</v>
       </c>
@@ -1736,7 +1756,7 @@
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
     </row>
-    <row r="2" spans="1:7" ht="19">
+    <row r="2" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -1750,7 +1770,7 @@
         <v>16</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>22</v>
@@ -1759,45 +1779,54 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>47</v>
+      </c>
+      <c r="E4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>86</v>
-      </c>
       <c r="B6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -1812,21 +1841,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
+      <selection pane="bottomLeft" activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.5" customWidth="1"/>
     <col min="2" max="2" width="20.5" customWidth="1"/>
     <col min="3" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="24.5" customWidth="1"/>
-    <col min="6" max="13" width="13" customWidth="1"/>
+    <col min="6" max="8" width="13" customWidth="1"/>
+    <col min="9" max="9" width="40.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="26">
+    <row r="1" spans="1:13" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>12</v>
       </c>
@@ -1843,7 +1874,7 @@
       <c r="L1" s="9"/>
       <c r="M1" s="9"/>
     </row>
-    <row r="2" spans="1:13" ht="19">
+    <row r="2" spans="1:13" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -1884,17 +1915,17 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F3" s="3">
         <v>1</v>
@@ -1903,23 +1934,26 @@
         <v>1</v>
       </c>
       <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
+      <c r="I3" s="3" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A3 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B3 &amp; ")"</f>
+        <v>power:GeneratingUnit(power:name)</v>
+      </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F4" s="3">
         <v>1</v>
@@ -1928,23 +1962,26 @@
         <v>1</v>
       </c>
       <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
+      <c r="I4" s="3" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A4 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B4 &amp; ")"</f>
+        <v>power:GeneratingUnit(power:type)</v>
+      </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1953,23 +1990,26 @@
         <v>1</v>
       </c>
       <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
+      <c r="I5" s="3" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A5 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B5 &amp; ")"</f>
+        <v>power:GeneratingUnit(power:activePower)</v>
+      </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F6" s="3">
         <v>0</v>
@@ -1978,13 +2018,16 @@
         <v>1</v>
       </c>
       <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+      <c r="I6" s="3" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A6 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B6 &amp; ")"</f>
+        <v>power:GeneratingUnit(power:geoLocation)</v>
+      </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1999,17 +2042,17 @@
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F8" s="4">
         <v>0</v>
@@ -2018,23 +2061,26 @@
         <v>1</v>
       </c>
       <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+      <c r="I8" s="4" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A8 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B8 &amp; ")"</f>
+        <v>power:WindTurbine(power:manufacturer)</v>
+      </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F9" s="4">
         <v>1</v>
@@ -2043,23 +2089,26 @@
         <v>1</v>
       </c>
       <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
+      <c r="I9" s="4" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A9 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B9 &amp; ")"</f>
+        <v>power:WindTurbine(power:ratedPower)</v>
+      </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F10" s="4">
         <v>1</v>
@@ -2068,23 +2117,26 @@
         <v>1</v>
       </c>
       <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
+      <c r="I10" s="4" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A10 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B10 &amp; ")"</f>
+        <v>power:WindTurbine(power:hubHeight)</v>
+      </c>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F11" s="4">
         <v>0</v>
@@ -2093,23 +2145,26 @@
         <v>1</v>
       </c>
       <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
+      <c r="I11" s="4" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A11 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B11 &amp; ")"</f>
+        <v>power:WindTurbine(power:arrayCableConnection)</v>
+      </c>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F12" s="4">
         <v>0</v>
@@ -2118,13 +2173,16 @@
         <v>1</v>
       </c>
       <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
+      <c r="I12" s="4" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A12 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B12 &amp; ")"</f>
+        <v>power:WindTurbine(power:lifeExpectancy)</v>
+      </c>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -2139,17 +2197,17 @@
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F14" s="3">
         <v>1</v>
@@ -2158,23 +2216,26 @@
         <v>1</v>
       </c>
       <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
+      <c r="I14" s="3" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A14 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B14 &amp; ")"</f>
+        <v>power:EnergyArea(power:name)</v>
+      </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F15" s="3">
         <v>0</v>
@@ -2183,23 +2244,26 @@
         <v>1</v>
       </c>
       <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
+      <c r="I15" s="3" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A15 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B15 &amp; ")"</f>
+        <v>power:EnergyArea(power:geoLocation)</v>
+      </c>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F16" s="3">
         <v>1</v>
@@ -2208,23 +2272,26 @@
         <v>1</v>
       </c>
       <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
+      <c r="I16" s="3" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A16 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B16 &amp; ")"</f>
+        <v>power:EnergyArea(power:ratedPower)</v>
+      </c>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F17" s="3">
         <v>1</v>
@@ -2233,13 +2300,16 @@
         <v>1</v>
       </c>
       <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
+      <c r="I17" s="3" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A17 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B17 &amp; ")"</f>
+        <v>power:EnergyArea(power:activePower)</v>
+      </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -2254,17 +2324,17 @@
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F19" s="4">
         <v>0</v>
@@ -2273,23 +2343,26 @@
         <v>1</v>
       </c>
       <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
+      <c r="I19" s="4" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A19 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B19 &amp; ")"</f>
+        <v>power:WindFarm(power:substation)</v>
+      </c>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F20" s="4">
         <v>0</v>
@@ -2298,59 +2371,68 @@
         <v>1</v>
       </c>
       <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
+      <c r="I20" s="4" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A20 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B20 &amp; ")"</f>
+        <v>power:WindFarm(power:exportCable)</v>
+      </c>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F21" s="4">
         <v>0</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
+      <c r="I21" s="4" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A21 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B21 &amp; ")"</f>
+        <v>power:WindFarm(power:arrayCable)</v>
+      </c>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F22" s="4">
         <v>0</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
+      <c r="I22" s="4" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A22 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B22 &amp; ")"</f>
+        <v>power:WindFarm(power:windTurbines)</v>
+      </c>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -2365,17 +2447,17 @@
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F24" s="3">
         <v>1</v>
@@ -2384,23 +2466,26 @@
         <v>1</v>
       </c>
       <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
+      <c r="I24" s="3" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A24 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B24 &amp; ")"</f>
+        <v>power:Substation(power:name)</v>
+      </c>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F25" s="3">
         <v>0</v>
@@ -2409,23 +2494,26 @@
         <v>1</v>
       </c>
       <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
+      <c r="I25" s="3" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A25 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B25 &amp; ")"</f>
+        <v>power:Substation(power:location)</v>
+      </c>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F26" s="3">
         <v>0</v>
@@ -2434,23 +2522,26 @@
         <v>1</v>
       </c>
       <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
+      <c r="I26" s="3" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A26 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B26 &amp; ")"</f>
+        <v>power:Substation(power:mainTransformer)</v>
+      </c>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F27" s="3">
         <v>0</v>
@@ -2459,23 +2550,26 @@
         <v>1</v>
       </c>
       <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
+      <c r="I27" s="3" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A27 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B27 &amp; ")"</f>
+        <v>power:Substation(power:primaryPowerLine)</v>
+      </c>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F28" s="3">
         <v>0</v>
@@ -2484,23 +2578,26 @@
         <v>1</v>
       </c>
       <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
+      <c r="I28" s="3" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A28 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B28 &amp; ")"</f>
+        <v>power:Substation(power:secondaryPowerLine)</v>
+      </c>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F29" s="3">
         <v>1</v>
@@ -2509,23 +2606,26 @@
         <v>1</v>
       </c>
       <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
+      <c r="I29" s="3" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A29 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B29 &amp; ")"</f>
+        <v>power:Substation(power:primaryVoltage)</v>
+      </c>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F30" s="3">
         <v>1</v>
@@ -2534,82 +2634,94 @@
         <v>1</v>
       </c>
       <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
+      <c r="I30" s="3" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A30 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B30 &amp; ")"</f>
+        <v>power:Substation(power:secondaryVoltage)</v>
+      </c>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F31" s="3">
         <v>0</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
+      <c r="I31" s="3" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A31 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B31 &amp; ")"</f>
+        <v>power:Substation(power:circuitBreaker)</v>
+      </c>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F32" s="3">
         <v>0</v>
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
+      <c r="I32" s="3" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A32 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B32 &amp; ")"</f>
+        <v>power:Substation(power:disconnectSwitch)</v>
+      </c>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F33" s="3">
         <v>0</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
+      <c r="I33" s="3" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A33 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B33 &amp; ")"</f>
+        <v>power:Substation(power:currentTransformer)</v>
+      </c>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -2624,17 +2736,17 @@
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>72</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F35" s="4">
         <v>0</v>
@@ -2649,17 +2761,17 @@
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F36" s="4">
         <v>0</v>
@@ -2674,17 +2786,17 @@
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F37" s="4">
         <v>1</v>
@@ -2699,17 +2811,17 @@
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F38" s="4">
         <v>0</v>
@@ -2724,7 +2836,7 @@
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -2739,17 +2851,17 @@
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>78</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F40" s="3">
         <v>0</v>
@@ -2764,17 +2876,17 @@
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F41" s="3">
         <v>1</v>
@@ -2789,17 +2901,17 @@
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F42" s="3">
         <v>0</v>
@@ -2812,7 +2924,7 @@
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -2827,17 +2939,17 @@
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F44" s="4">
         <v>1</v>
@@ -2852,17 +2964,17 @@
       <c r="L44" s="4"/>
       <c r="M44" s="4"/>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F45" s="4">
         <v>0</v>
@@ -2877,17 +2989,17 @@
       <c r="L45" s="4"/>
       <c r="M45" s="4"/>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B46" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>84</v>
       </c>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
       <c r="E46" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F46" s="4">
         <v>1</v>
@@ -2902,7 +3014,7 @@
       <c r="L46" s="4"/>
       <c r="M46" s="4"/>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -2917,17 +3029,17 @@
       <c r="L47" s="4"/>
       <c r="M47" s="4"/>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F48" s="3">
         <v>1</v>
@@ -2942,7 +3054,7 @@
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -2957,17 +3069,17 @@
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B50" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
       <c r="E50" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F50" s="4">
         <v>1</v>
@@ -2982,17 +3094,17 @@
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
       <c r="E51" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F51" s="4">
         <v>1</v>
@@ -3007,7 +3119,7 @@
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -3022,17 +3134,17 @@
       <c r="L52" s="4"/>
       <c r="M52" s="4"/>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B53" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>90</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
       <c r="E53" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F53" s="3">
         <v>0</v>
@@ -3045,7 +3157,7 @@
       <c r="L53" s="3"/>
       <c r="M53" s="3"/>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -3060,17 +3172,17 @@
       <c r="L54" s="3"/>
       <c r="M54" s="3"/>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
       <c r="E55" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F55" s="4">
         <v>0</v>
@@ -3083,7 +3195,7 @@
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -3098,17 +3210,17 @@
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B57" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
       <c r="E57" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F57" s="3">
         <v>0</v>
@@ -3123,7 +3235,7 @@
       <c r="L57" s="3"/>
       <c r="M57" s="3"/>
     </row>
-    <row r="58" spans="1:13">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -3138,17 +3250,17 @@
       <c r="L58" s="3"/>
       <c r="M58" s="3"/>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
       <c r="E59" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F59" s="4">
         <v>0</v>
@@ -3163,7 +3275,7 @@
       <c r="L59" s="4"/>
       <c r="M59" s="4"/>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -3178,17 +3290,17 @@
       <c r="L60" s="4"/>
       <c r="M60" s="4"/>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
       <c r="E61" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F61" s="3">
         <v>0</v>
@@ -3203,7 +3315,7 @@
       <c r="L61" s="3"/>
       <c r="M61" s="3"/>
     </row>
-    <row r="62" spans="1:13">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -3218,17 +3330,17 @@
       <c r="L62" s="3"/>
       <c r="M62" s="3"/>
     </row>
-    <row r="63" spans="1:13">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B63" s="4" t="s">
         <v>96</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>97</v>
       </c>
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
       <c r="E63" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F63" s="4">
         <v>1</v>
@@ -3243,7 +3355,7 @@
       <c r="L63" s="4"/>
       <c r="M63" s="4"/>
     </row>
-    <row r="64" spans="1:13">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
@@ -3258,17 +3370,17 @@
       <c r="L64" s="4"/>
       <c r="M64" s="4"/>
     </row>
-    <row r="65" spans="1:13">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B65" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>99</v>
       </c>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
       <c r="E65" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F65" s="3">
         <v>0</v>
@@ -3283,17 +3395,17 @@
       <c r="L65" s="3"/>
       <c r="M65" s="3"/>
     </row>
-    <row r="66" spans="1:13">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
       <c r="E66" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F66" s="3">
         <v>0</v>
@@ -3313,6 +3425,7 @@
     <mergeCell ref="A1:M1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -3320,18 +3433,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C59" sqref="C59"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="7" width="13" customWidth="1"/>
+    <col min="3" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" customWidth="1"/>
+    <col min="6" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26">
+    <row r="1" spans="1:7" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>26</v>
       </c>
@@ -3342,7 +3457,7 @@
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
     </row>
-    <row r="2" spans="1:7" ht="19">
+    <row r="2" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -3356,7 +3471,7 @@
         <v>16</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>22</v>
@@ -3365,176 +3480,280 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>28</v>
+      </c>
+      <c r="E3" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A3</f>
+        <v>power:GeneratingUnit</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>28</v>
+      </c>
+      <c r="E4" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A4</f>
+        <v>power:WindTurbine</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>45</v>
+      </c>
+      <c r="E5" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A5</f>
+        <v>power:EnergyArea</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>45</v>
+      </c>
+      <c r="E6" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A6</f>
+        <v>power:WindFarm</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>55</v>
+      </c>
+      <c r="E7" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A7</f>
+        <v>power:Substation</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A8</f>
+        <v>power:OffshoreSubstation</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>101</v>
       </c>
-      <c r="B8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A9</f>
+        <v>power:TransmissionSubstation</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>102</v>
       </c>
-      <c r="B9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A10</f>
+        <v>power:DistributionSubstation</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>103</v>
       </c>
-      <c r="B10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E11" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A11</f>
+        <v>power:OnshoreSubstation</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A12</f>
+        <v>power:PowerLine</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>104</v>
       </c>
-      <c r="B11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A13</f>
+        <v>power:ArrayCable</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>105</v>
       </c>
-      <c r="B13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A14</f>
+        <v>power:ExportCable</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>106</v>
       </c>
-      <c r="B14" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A15</f>
+        <v>power:Transmission</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>107</v>
       </c>
-      <c r="B15" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A16</f>
+        <v>power:DistributionLine</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A17</f>
+        <v>power:Meter</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>82</v>
+      </c>
+      <c r="E18" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A18</f>
+        <v>power:EnergyConsumer</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>108</v>
       </c>
-      <c r="B16" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>109</v>
-      </c>
       <c r="B19" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>82</v>
+      </c>
+      <c r="E19" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A19</f>
+        <v>power:ElectricCarCharger</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E20" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A20</f>
+        <v>power:GeoLocation</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>86</v>
-      </c>
       <c r="B21" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>84</v>
+      </c>
+      <c r="E21" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A21</f>
+        <v>power:Point</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B22" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>84</v>
+      </c>
+      <c r="E22" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A22</f>
+        <v>power:MultiLineString</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" t="s">
+        <v>84</v>
+      </c>
+      <c r="E23" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A23</f>
+        <v>power:Polygon</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>91</v>
       </c>
-      <c r="B23" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="E24" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A24</f>
+        <v>power:CircuitBreaker</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>93</v>
+      </c>
+      <c r="E25" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A25</f>
+        <v>power:CurrentTransformer</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
+      <c r="E26" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A26</f>
+        <v>power:DisconnectSwitch</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="E27" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A27</f>
+        <v>power:VoltageLevel</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>98</v>
+        <v>97</v>
+      </c>
+      <c r="E28" t="str">
+        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A28</f>
+        <v>power:VoltageTransformer</v>
       </c>
     </row>
   </sheetData>
@@ -3549,17 +3768,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16">
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3567,60 +3786,60 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16">
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="16">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="16">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="16">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="16">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="16">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="16">
+    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="16">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -3628,7 +3847,7 @@
         <v>45377.41672594368</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="16">
+    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -3636,12 +3855,12 @@
         <v>45377.41672594368</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="16">
+    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: small bug in sheet
</commit_message>
<xml_diff>
--- a/docs/artifacts/rules/information-analytics-olav.xlsx
+++ b/docs/artifacts/rules/information-analytics-olav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\artifacts\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4BAACB-7BCF-4D7F-B0C3-F3AEDC55BCE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A313EF-B9A8-4346-9BDE-7862A36F3900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17340" yWindow="0" windowWidth="24036" windowHeight="16656" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="205">
   <si>
     <t>role</t>
   </si>
   <si>
     <t>information architect</t>
-  </si>
-  <si>
-    <t>schema_</t>
   </si>
   <si>
     <t>extension</t>
@@ -742,12 +739,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1053,8 +1050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA13" sqref="AA13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1073,79 +1070,79 @@
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>166</v>
       </c>
       <c r="B2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>178</v>
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7">
         <v>45377</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="9">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7">
         <v>45331</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -1160,7 +1157,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
     </sheetView>
@@ -1177,232 +1174,232 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
+      <c r="A1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
     </row>
     <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
         <v>29</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
         <v>31</v>
-      </c>
-      <c r="E4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="I4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
         <v>33</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
         <v>34</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="I5" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
         <v>36</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="I6" t="s">
         <v>37</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="I6" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s">
         <v>39</v>
       </c>
-      <c r="B7" t="s">
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
         <v>40</v>
-      </c>
-      <c r="E7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="I7" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" t="s">
         <v>42</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="I8" t="s">
         <v>43</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="I8" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="I9" t="s">
         <v>45</v>
-      </c>
-      <c r="E9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="I9" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" t="s">
         <v>50</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="I10" t="s">
         <v>51</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="I10" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1410,13 +1407,13 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -1427,13 +1424,13 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1444,13 +1441,13 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -1461,13 +1458,13 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -1476,18 +1473,18 @@
         <v>1</v>
       </c>
       <c r="I16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -1496,35 +1493,35 @@
         <v>1</v>
       </c>
       <c r="I17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F18">
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -1532,13 +1529,13 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B20" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E20" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -1546,13 +1543,13 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B21" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -1563,13 +1560,13 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -1580,13 +1577,13 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -1597,13 +1594,13 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -1614,13 +1611,13 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -1631,13 +1628,13 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B27" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -1648,13 +1645,13 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B28" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E28" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -1665,13 +1662,13 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B29" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -1682,13 +1679,13 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B30" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -1699,13 +1696,13 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B31" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -1716,13 +1713,13 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B32" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F32">
         <v>0</v>
@@ -1733,13 +1730,13 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B33" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F33">
         <v>0</v>
@@ -1750,13 +1747,13 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B34" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -1767,13 +1764,13 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B36" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -1784,13 +1781,13 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B37" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -1801,13 +1798,13 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B38" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -1815,13 +1812,13 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B39" t="s">
+        <v>202</v>
+      </c>
+      <c r="E39" t="s">
         <v>203</v>
-      </c>
-      <c r="E39" t="s">
-        <v>204</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -1832,13 +1829,13 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B40" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F40">
         <v>1</v>
@@ -1871,87 +1868,87 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="A1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
     </row>
     <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="E2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="G2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -1983,74 +1980,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
+      <c r="A1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
     </row>
     <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F3" s="3">
         <v>1</v>
@@ -2060,7 +2057,7 @@
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -2069,15 +2066,15 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F4" s="3">
         <v>1</v>
@@ -2087,7 +2084,7 @@
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
@@ -2096,15 +2093,15 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -2114,7 +2111,7 @@
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -2123,15 +2120,15 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F6" s="3">
         <v>0</v>
@@ -2141,7 +2138,7 @@
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -2165,15 +2162,15 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F8" s="4">
         <v>0</v>
@@ -2183,7 +2180,7 @@
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
@@ -2192,15 +2189,15 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F9" s="4">
         <v>1</v>
@@ -2210,7 +2207,7 @@
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
@@ -2219,15 +2216,15 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F10" s="4">
         <v>1</v>
@@ -2237,7 +2234,7 @@
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
@@ -2246,15 +2243,15 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F11" s="4">
         <v>0</v>
@@ -2264,7 +2261,7 @@
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
@@ -2273,15 +2270,15 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F12" s="4">
         <v>0</v>
@@ -2291,7 +2288,7 @@
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
@@ -2315,15 +2312,15 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F14" s="3">
         <v>1</v>
@@ -2333,7 +2330,7 @@
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -2342,15 +2339,15 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F15" s="3">
         <v>0</v>
@@ -2360,7 +2357,7 @@
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -2369,15 +2366,15 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F16" s="3">
         <v>1</v>
@@ -2387,7 +2384,7 @@
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
@@ -2396,15 +2393,15 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F17" s="3">
         <v>1</v>
@@ -2414,7 +2411,7 @@
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
@@ -2438,15 +2435,15 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F19" s="4">
         <v>0</v>
@@ -2456,7 +2453,7 @@
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
@@ -2465,15 +2462,15 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F20" s="4">
         <v>0</v>
@@ -2483,7 +2480,7 @@
       </c>
       <c r="H20" s="4"/>
       <c r="I20" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
@@ -2492,15 +2489,15 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F21" s="4">
         <v>0</v>
@@ -2508,7 +2505,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
@@ -2517,15 +2514,15 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F22" s="4">
         <v>0</v>
@@ -2533,7 +2530,7 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
@@ -2557,15 +2554,15 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F24" s="3">
         <v>1</v>
@@ -2575,7 +2572,7 @@
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
@@ -2584,15 +2581,15 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F25" s="3">
         <v>0</v>
@@ -2602,7 +2599,7 @@
       </c>
       <c r="H25" s="3"/>
       <c r="I25" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
@@ -2611,15 +2608,15 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F26" s="3">
         <v>0</v>
@@ -2629,7 +2626,7 @@
       </c>
       <c r="H26" s="3"/>
       <c r="I26" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
@@ -2638,15 +2635,15 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F27" s="3">
         <v>0</v>
@@ -2656,7 +2653,7 @@
       </c>
       <c r="H27" s="3"/>
       <c r="I27" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
@@ -2665,15 +2662,15 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F28" s="3">
         <v>0</v>
@@ -2683,7 +2680,7 @@
       </c>
       <c r="H28" s="3"/>
       <c r="I28" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
@@ -2692,15 +2689,15 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F29" s="3">
         <v>1</v>
@@ -2710,7 +2707,7 @@
       </c>
       <c r="H29" s="3"/>
       <c r="I29" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
@@ -2719,15 +2716,15 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F30" s="3">
         <v>1</v>
@@ -2737,7 +2734,7 @@
       </c>
       <c r="H30" s="3"/>
       <c r="I30" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
@@ -2746,15 +2743,15 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F31" s="3">
         <v>0</v>
@@ -2762,7 +2759,7 @@
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
@@ -2771,15 +2768,15 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F32" s="3">
         <v>0</v>
@@ -2787,7 +2784,7 @@
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
       <c r="I32" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
@@ -2796,15 +2793,15 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F33" s="3">
         <v>0</v>
@@ -2812,7 +2809,7 @@
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="I33" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
@@ -2836,15 +2833,15 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>96</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>97</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F35" s="4">
         <v>0</v>
@@ -2854,7 +2851,7 @@
       </c>
       <c r="H35" s="4"/>
       <c r="I35" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
@@ -2863,15 +2860,15 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F36" s="4">
         <v>0</v>
@@ -2881,7 +2878,7 @@
       </c>
       <c r="H36" s="4"/>
       <c r="I36" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
@@ -2890,15 +2887,15 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F37" s="4">
         <v>1</v>
@@ -2908,7 +2905,7 @@
       </c>
       <c r="H37" s="4"/>
       <c r="I37" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
@@ -2917,15 +2914,15 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F38" s="4">
         <v>0</v>
@@ -2935,7 +2932,7 @@
       </c>
       <c r="H38" s="4"/>
       <c r="I38" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
@@ -2959,15 +2956,15 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F40" s="3">
         <v>0</v>
@@ -2977,7 +2974,7 @@
       </c>
       <c r="H40" s="3"/>
       <c r="I40" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
@@ -2986,15 +2983,15 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F41" s="3">
         <v>1</v>
@@ -3004,7 +3001,7 @@
       </c>
       <c r="H41" s="3"/>
       <c r="I41" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
@@ -3013,15 +3010,15 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F42" s="3">
         <v>0</v>
@@ -3029,7 +3026,7 @@
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
       <c r="I42" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
@@ -3053,15 +3050,15 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F44" s="4">
         <v>1</v>
@@ -3071,7 +3068,7 @@
       </c>
       <c r="H44" s="4"/>
       <c r="I44" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
@@ -3080,15 +3077,15 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F45" s="4">
         <v>0</v>
@@ -3098,7 +3095,7 @@
       </c>
       <c r="H45" s="4"/>
       <c r="I45" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
@@ -3107,15 +3104,15 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
       <c r="E46" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F46" s="4">
         <v>1</v>
@@ -3125,7 +3122,7 @@
       </c>
       <c r="H46" s="4"/>
       <c r="I46" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
@@ -3149,15 +3146,15 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F48" s="3">
         <v>1</v>
@@ -3167,7 +3164,7 @@
       </c>
       <c r="H48" s="3"/>
       <c r="I48" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J48" s="3"/>
       <c r="K48" s="3"/>
@@ -3191,15 +3188,15 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B50" s="4" t="s">
         <v>122</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>123</v>
       </c>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
       <c r="E50" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F50" s="4">
         <v>1</v>
@@ -3209,7 +3206,7 @@
       </c>
       <c r="H50" s="4"/>
       <c r="I50" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
@@ -3218,15 +3215,15 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
       <c r="E51" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F51" s="4">
         <v>1</v>
@@ -3236,7 +3233,7 @@
       </c>
       <c r="H51" s="4"/>
       <c r="I51" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
@@ -3260,15 +3257,15 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B53" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>128</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
       <c r="E53" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F53" s="3">
         <v>0</v>
@@ -3276,7 +3273,7 @@
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
       <c r="I53" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
@@ -3300,15 +3297,15 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
       <c r="E55" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F55" s="4">
         <v>0</v>
@@ -3316,7 +3313,7 @@
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
       <c r="I55" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
@@ -3340,15 +3337,15 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B57" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>133</v>
       </c>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
       <c r="E57" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F57" s="3">
         <v>0</v>
@@ -3358,7 +3355,7 @@
       </c>
       <c r="H57" s="3"/>
       <c r="I57" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
@@ -3382,15 +3379,15 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
       <c r="E59" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F59" s="4">
         <v>0</v>
@@ -3400,7 +3397,7 @@
       </c>
       <c r="H59" s="4"/>
       <c r="I59" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
@@ -3424,15 +3421,15 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
       <c r="E61" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F61" s="3">
         <v>0</v>
@@ -3442,7 +3439,7 @@
       </c>
       <c r="H61" s="3"/>
       <c r="I61" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J61" s="3"/>
       <c r="K61" s="3"/>
@@ -3466,15 +3463,15 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B63" s="4" t="s">
         <v>139</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>140</v>
       </c>
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
       <c r="E63" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F63" s="4">
         <v>1</v>
@@ -3484,7 +3481,7 @@
       </c>
       <c r="H63" s="4"/>
       <c r="I63" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J63" s="4"/>
       <c r="K63" s="4"/>
@@ -3508,15 +3505,15 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B65" s="3" t="s">
         <v>142</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>143</v>
       </c>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
       <c r="E65" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F65" s="3">
         <v>0</v>
@@ -3526,7 +3523,7 @@
       </c>
       <c r="H65" s="3"/>
       <c r="I65" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J65" s="3"/>
       <c r="K65" s="3"/>
@@ -3535,15 +3532,15 @@
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
       <c r="E66" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F66" s="3">
         <v>0</v>
@@ -3553,7 +3550,7 @@
       </c>
       <c r="H66" s="3"/>
       <c r="I66" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J66" s="3"/>
       <c r="K66" s="3"/>
@@ -3586,287 +3583,287 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="A1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
     </row>
     <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="E2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="G2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>151</v>
+      </c>
+      <c r="B9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" t="s">
         <v>152</v>
-      </c>
-      <c r="B9" t="s">
-        <v>71</v>
-      </c>
-      <c r="E9" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>153</v>
+      </c>
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" t="s">
         <v>154</v>
-      </c>
-      <c r="B10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E10" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>155</v>
+      </c>
+      <c r="B11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E11" t="s">
         <v>156</v>
-      </c>
-      <c r="B11" t="s">
-        <v>152</v>
-      </c>
-      <c r="E11" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>159</v>
+      </c>
+      <c r="B15" t="s">
+        <v>95</v>
+      </c>
+      <c r="E15" t="s">
         <v>160</v>
-      </c>
-      <c r="B15" t="s">
-        <v>96</v>
-      </c>
-      <c r="E15" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -3899,60 +3896,60 @@
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B2" t="s">
         <v>167</v>
-      </c>
-      <c r="B2" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B6" t="s">
         <v>172</v>
-      </c>
-      <c r="B6" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="5">
         <v>45388.62510806237</v>
@@ -3960,7 +3957,7 @@
     </row>
     <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="5">
         <v>45388.62510806237</v>
@@ -3968,10 +3965,10 @@
     </row>
     <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Olav with references (#370)
* refactor: Update Olav with references

* fix: small bug in sheet

* tests: updated
</commit_message>
<xml_diff>
--- a/docs/artifacts/rules/information-analytics-olav.xlsx
+++ b/docs/artifacts/rules/information-analytics-olav.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Secondary/repos/neat/docs/artifacts/rules/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\artifacts\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7179DD1F-DDFC-124D-80AF-6E33644A197D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A313EF-B9A8-4346-9BDE-7862A36F3900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -20,24 +20,12 @@
     <sheet name="RefClasses" sheetId="5" r:id="rId5"/>
     <sheet name="RefMetadata" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="205">
   <si>
     <t>role</t>
   </si>
@@ -45,339 +33,516 @@
     <t>information architect</t>
   </si>
   <si>
+    <t>extension</t>
+  </si>
+  <si>
+    <t>prefix</t>
+  </si>
+  <si>
+    <t>namespace</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>created</t>
+  </si>
+  <si>
+    <t>updated</t>
+  </si>
+  <si>
+    <t>creator</t>
+  </si>
+  <si>
+    <t>Definition of Properties per Class</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Property</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Value Type</t>
+  </si>
+  <si>
+    <t>Min Count</t>
+  </si>
+  <si>
+    <t>Max Count</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Match Type</t>
+  </si>
+  <si>
+    <t>Rule Type</t>
+  </si>
+  <si>
+    <t>Rule</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Definition of Classes</t>
+  </si>
+  <si>
+    <t>Parent Class</t>
+  </si>
+  <si>
+    <t>GeneratingUnit</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>power:GeneratingUnit(property=name)</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>power:GeneratingUnit(property=type)</t>
+  </si>
+  <si>
+    <t>activePower</t>
+  </si>
+  <si>
+    <t>timeseries</t>
+  </si>
+  <si>
+    <t>power:GeneratingUnit(property=activePower)</t>
+  </si>
+  <si>
+    <t>geoLocation</t>
+  </si>
+  <si>
+    <t>power:Point</t>
+  </si>
+  <si>
+    <t>power:GeneratingUnit(property=geoLocation)</t>
+  </si>
+  <si>
+    <t>WindTurbine</t>
+  </si>
+  <si>
+    <t>manufacturer</t>
+  </si>
+  <si>
+    <t>power:WindTurbine(property=manufacturer)</t>
+  </si>
+  <si>
+    <t>ratedPower</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>power:WindTurbine(property=ratedPower)</t>
+  </si>
+  <si>
+    <t>hubHeight</t>
+  </si>
+  <si>
+    <t>power:WindTurbine(property=hubHeight)</t>
+  </si>
+  <si>
+    <t>arrayCableConnection</t>
+  </si>
+  <si>
+    <t>power:ArrayCable</t>
+  </si>
+  <si>
+    <t>power:WindTurbine(property=arrayCableConnection)</t>
+  </si>
+  <si>
+    <t>lifeExpectancy</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>power:WindTurbine(property=lifeExpectancy)</t>
+  </si>
+  <si>
+    <t>EnergyArea</t>
+  </si>
+  <si>
+    <t>power:EnergyArea(property=name)</t>
+  </si>
+  <si>
+    <t>power:Polygon</t>
+  </si>
+  <si>
+    <t>power:EnergyArea(property=geoLocation)</t>
+  </si>
+  <si>
+    <t>power:EnergyArea(property=ratedPower)</t>
+  </si>
+  <si>
+    <t>power:EnergyArea(property=activePower)</t>
+  </si>
+  <si>
+    <t>WindFarm</t>
+  </si>
+  <si>
+    <t>substation</t>
+  </si>
+  <si>
+    <t>power:OffshoreSubstation</t>
+  </si>
+  <si>
+    <t>power:WindFarm(property=substation)</t>
+  </si>
+  <si>
+    <t>exportCable</t>
+  </si>
+  <si>
+    <t>power:ExportCable</t>
+  </si>
+  <si>
+    <t>power:WindFarm(property=exportCable)</t>
+  </si>
+  <si>
+    <t>arrayCable</t>
+  </si>
+  <si>
+    <t>power:WindFarm(property=arrayCable)</t>
+  </si>
+  <si>
+    <t>windTurbines</t>
+  </si>
+  <si>
+    <t>power:WindTurbine</t>
+  </si>
+  <si>
+    <t>power:WindFarm(property=windTurbines)</t>
+  </si>
+  <si>
+    <t>Substation</t>
+  </si>
+  <si>
+    <t>power:Substation(property=name)</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>power:Substation(property=location)</t>
+  </si>
+  <si>
+    <t>mainTransformer</t>
+  </si>
+  <si>
+    <t>power:VoltageTransformer</t>
+  </si>
+  <si>
+    <t>power:Substation(property=mainTransformer)</t>
+  </si>
+  <si>
+    <t>primaryPowerLine</t>
+  </si>
+  <si>
+    <t>power:PowerLine</t>
+  </si>
+  <si>
+    <t>power:Substation(property=primaryPowerLine)</t>
+  </si>
+  <si>
+    <t>secondaryPowerLine</t>
+  </si>
+  <si>
+    <t>power:Substation(property=secondaryPowerLine)</t>
+  </si>
+  <si>
+    <t>primaryVoltage</t>
+  </si>
+  <si>
+    <t>power:Substation(property=primaryVoltage)</t>
+  </si>
+  <si>
+    <t>secondaryVoltage</t>
+  </si>
+  <si>
+    <t>power:Substation(property=secondaryVoltage)</t>
+  </si>
+  <si>
+    <t>circuitBreaker</t>
+  </si>
+  <si>
+    <t>power:CircuitBreaker</t>
+  </si>
+  <si>
+    <t>power:Substation(property=circuitBreaker)</t>
+  </si>
+  <si>
+    <t>disconnectSwitch</t>
+  </si>
+  <si>
+    <t>power:DisconnectSwitch</t>
+  </si>
+  <si>
+    <t>power:Substation(property=disconnectSwitch)</t>
+  </si>
+  <si>
+    <t>currentTransformer</t>
+  </si>
+  <si>
+    <t>power:CurrentTransformer</t>
+  </si>
+  <si>
+    <t>power:Substation(property=currentTransformer)</t>
+  </si>
+  <si>
+    <t>PowerLine</t>
+  </si>
+  <si>
+    <t>voltageLevel</t>
+  </si>
+  <si>
+    <t>power:VoltageLevel</t>
+  </si>
+  <si>
+    <t>power:PowerLine(property=voltageLevel)</t>
+  </si>
+  <si>
+    <t>power:MultiLineString</t>
+  </si>
+  <si>
+    <t>power:PowerLine(property=geoLocation)</t>
+  </si>
+  <si>
+    <t>currentVoltage</t>
+  </si>
+  <si>
+    <t>power:PowerLine(property=currentVoltage)</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>power:PowerLine(property=length)</t>
+  </si>
+  <si>
+    <t>Meter</t>
+  </si>
+  <si>
+    <t>powerLine</t>
+  </si>
+  <si>
+    <t>power:DistributionLine</t>
+  </si>
+  <si>
+    <t>power:Meter(property=powerLine)</t>
+  </si>
+  <si>
+    <t>consumption</t>
+  </si>
+  <si>
+    <t>power:Meter(property=consumption)</t>
+  </si>
+  <si>
+    <t>consumer</t>
+  </si>
+  <si>
+    <t>power:ElectricCarCharger</t>
+  </si>
+  <si>
+    <t>power:Meter(property=consumer)</t>
+  </si>
+  <si>
+    <t>EnergyConsumer</t>
+  </si>
+  <si>
+    <t>power:EnergyConsumer(property=name)</t>
+  </si>
+  <si>
+    <t>power:EnergyConsumer(property=location)</t>
+  </si>
+  <si>
+    <t>load</t>
+  </si>
+  <si>
+    <t>power:EnergyConsumer(property=load)</t>
+  </si>
+  <si>
+    <t>GeoLocation</t>
+  </si>
+  <si>
+    <t>power:GeoLocation(property=name)</t>
+  </si>
+  <si>
+    <t>Point</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>power:Point(property=latitude)</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>power:Point(property=longitude)</t>
+  </si>
+  <si>
+    <t>MultiLineString</t>
+  </si>
+  <si>
+    <t>point</t>
+  </si>
+  <si>
+    <t>power:MultiLineString(property=point)</t>
+  </si>
+  <si>
+    <t>Polygon</t>
+  </si>
+  <si>
+    <t>power:Polygon(property=point)</t>
+  </si>
+  <si>
+    <t>CircuitBreaker</t>
+  </si>
+  <si>
+    <t>maxCapacity</t>
+  </si>
+  <si>
+    <t>power:CircuitBreaker(property=maxCapacity)</t>
+  </si>
+  <si>
+    <t>CurrentTransformer</t>
+  </si>
+  <si>
+    <t>power:CurrentTransformer(property=maxCapacity)</t>
+  </si>
+  <si>
+    <t>DisconnectSwitch</t>
+  </si>
+  <si>
+    <t>power:DisconnectSwitch(property=maxCapacity)</t>
+  </si>
+  <si>
+    <t>VoltageLevel</t>
+  </si>
+  <si>
+    <t>maxLevel</t>
+  </si>
+  <si>
+    <t>power:VoltageLevel(property=maxLevel)</t>
+  </si>
+  <si>
+    <t>VoltageTransformer</t>
+  </si>
+  <si>
+    <t>outputVoltageLevel</t>
+  </si>
+  <si>
+    <t>power:VoltageTransformer(property=outputVoltageLevel)</t>
+  </si>
+  <si>
+    <t>inputVoltageLevel</t>
+  </si>
+  <si>
+    <t>power:VoltageTransformer(property=inputVoltageLevel)</t>
+  </si>
+  <si>
+    <t>power:GeneratingUnit</t>
+  </si>
+  <si>
+    <t>power:EnergyArea</t>
+  </si>
+  <si>
+    <t>power:WindFarm</t>
+  </si>
+  <si>
+    <t>power:Substation</t>
+  </si>
+  <si>
+    <t>OffshoreSubstation</t>
+  </si>
+  <si>
+    <t>TransmissionSubstation</t>
+  </si>
+  <si>
+    <t>power:TransmissionSubstation</t>
+  </si>
+  <si>
+    <t>DistributionSubstation</t>
+  </si>
+  <si>
+    <t>power:DistributionSubstation</t>
+  </si>
+  <si>
+    <t>OnshoreSubstation</t>
+  </si>
+  <si>
+    <t>power:OnshoreSubstation</t>
+  </si>
+  <si>
+    <t>ArrayCable</t>
+  </si>
+  <si>
+    <t>ExportCable</t>
+  </si>
+  <si>
+    <t>Transmission</t>
+  </si>
+  <si>
+    <t>power:Transmission</t>
+  </si>
+  <si>
+    <t>DistributionLine</t>
+  </si>
+  <si>
+    <t>power:Meter</t>
+  </si>
+  <si>
+    <t>power:EnergyConsumer</t>
+  </si>
+  <si>
+    <t>ElectricCarCharger</t>
+  </si>
+  <si>
+    <t>power:GeoLocation</t>
+  </si>
+  <si>
     <t>schema</t>
   </si>
   <si>
-    <t>extension</t>
-  </si>
-  <si>
-    <t>prefix</t>
-  </si>
-  <si>
-    <t>namespace</t>
+    <t>complete</t>
+  </si>
+  <si>
+    <t>addition</t>
+  </si>
+  <si>
+    <t>power</t>
+  </si>
+  <si>
+    <t>https://purl.orgl/neat/power/</t>
   </si>
   <si>
     <t>title</t>
   </si>
   <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>version</t>
-  </si>
-  <si>
-    <t>created</t>
-  </si>
-  <si>
-    <t>updated</t>
-  </si>
-  <si>
-    <t>creator</t>
-  </si>
-  <si>
-    <t>Definition of Properties per Class</t>
-  </si>
-  <si>
-    <t>Class</t>
-  </si>
-  <si>
-    <t>Property</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Value Type</t>
-  </si>
-  <si>
-    <t>Min Count</t>
-  </si>
-  <si>
-    <t>Max Count</t>
-  </si>
-  <si>
-    <t>Default</t>
-  </si>
-  <si>
-    <t>Reference</t>
-  </si>
-  <si>
-    <t>Match Type</t>
-  </si>
-  <si>
-    <t>Rule Type</t>
-  </si>
-  <si>
-    <t>Rule</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>Definition of Classes</t>
-  </si>
-  <si>
-    <t>Parent Class</t>
-  </si>
-  <si>
-    <t>GeneratingUnit</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>string</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>activePower</t>
-  </si>
-  <si>
-    <t>timeseries</t>
-  </si>
-  <si>
-    <t>geoLocation</t>
-  </si>
-  <si>
-    <t>power:Point</t>
-  </si>
-  <si>
-    <t>WindTurbine</t>
-  </si>
-  <si>
-    <t>manufacturer</t>
-  </si>
-  <si>
-    <t>ratedPower</t>
-  </si>
-  <si>
-    <t>double</t>
-  </si>
-  <si>
-    <t>hubHeight</t>
-  </si>
-  <si>
-    <t>arrayCableConnection</t>
-  </si>
-  <si>
-    <t>power:ArrayCable</t>
-  </si>
-  <si>
-    <t>lifeExpectancy</t>
-  </si>
-  <si>
-    <t>integer</t>
-  </si>
-  <si>
-    <t>EnergyArea</t>
-  </si>
-  <si>
-    <t>power:Polygon</t>
-  </si>
-  <si>
-    <t>WindFarm</t>
-  </si>
-  <si>
-    <t>substation</t>
-  </si>
-  <si>
-    <t>power:OffshoreSubstation</t>
-  </si>
-  <si>
-    <t>exportCable</t>
-  </si>
-  <si>
-    <t>power:ExportCable</t>
-  </si>
-  <si>
-    <t>arrayCable</t>
-  </si>
-  <si>
-    <t>windTurbines</t>
-  </si>
-  <si>
-    <t>power:WindTurbine</t>
-  </si>
-  <si>
-    <t>Substation</t>
-  </si>
-  <si>
-    <t>location</t>
-  </si>
-  <si>
-    <t>mainTransformer</t>
-  </si>
-  <si>
-    <t>power:VoltageTransformer</t>
-  </si>
-  <si>
-    <t>primaryPowerLine</t>
-  </si>
-  <si>
-    <t>power:PowerLine</t>
-  </si>
-  <si>
-    <t>secondaryPowerLine</t>
-  </si>
-  <si>
-    <t>primaryVoltage</t>
-  </si>
-  <si>
-    <t>secondaryVoltage</t>
-  </si>
-  <si>
-    <t>circuitBreaker</t>
-  </si>
-  <si>
-    <t>power:CircuitBreaker</t>
-  </si>
-  <si>
-    <t>disconnectSwitch</t>
-  </si>
-  <si>
-    <t>power:DisconnectSwitch</t>
-  </si>
-  <si>
-    <t>currentTransformer</t>
-  </si>
-  <si>
-    <t>power:CurrentTransformer</t>
-  </si>
-  <si>
-    <t>PowerLine</t>
-  </si>
-  <si>
-    <t>voltageLevel</t>
-  </si>
-  <si>
-    <t>power:VoltageLevel</t>
-  </si>
-  <si>
-    <t>power:MultiLineString</t>
-  </si>
-  <si>
-    <t>currentVoltage</t>
-  </si>
-  <si>
-    <t>length</t>
-  </si>
-  <si>
-    <t>Meter</t>
-  </si>
-  <si>
-    <t>powerLine</t>
-  </si>
-  <si>
-    <t>power:DistributionLine</t>
-  </si>
-  <si>
-    <t>consumption</t>
-  </si>
-  <si>
-    <t>consumer</t>
-  </si>
-  <si>
-    <t>power:ElectricCarCharger</t>
-  </si>
-  <si>
-    <t>EnergyConsumer</t>
-  </si>
-  <si>
-    <t>load</t>
-  </si>
-  <si>
-    <t>GeoLocation</t>
-  </si>
-  <si>
-    <t>Point</t>
-  </si>
-  <si>
-    <t>latitude</t>
-  </si>
-  <si>
-    <t>longitude</t>
-  </si>
-  <si>
-    <t>MultiLineString</t>
-  </si>
-  <si>
-    <t>point</t>
-  </si>
-  <si>
-    <t>Polygon</t>
-  </si>
-  <si>
-    <t>CircuitBreaker</t>
-  </si>
-  <si>
-    <t>maxCapacity</t>
-  </si>
-  <si>
-    <t>CurrentTransformer</t>
-  </si>
-  <si>
-    <t>DisconnectSwitch</t>
-  </si>
-  <si>
-    <t>VoltageLevel</t>
-  </si>
-  <si>
-    <t>maxLevel</t>
-  </si>
-  <si>
-    <t>VoltageTransformer</t>
-  </si>
-  <si>
-    <t>outputVoltageLevel</t>
-  </si>
-  <si>
-    <t>inputVoltageLevel</t>
-  </si>
-  <si>
-    <t>OffshoreSubstation</t>
-  </si>
-  <si>
-    <t>TransmissionSubstation</t>
-  </si>
-  <si>
-    <t>DistributionSubstation</t>
-  </si>
-  <si>
-    <t>OnshoreSubstation</t>
-  </si>
-  <si>
-    <t>ArrayCable</t>
-  </si>
-  <si>
-    <t>ExportCable</t>
-  </si>
-  <si>
-    <t>Transmission</t>
-  </si>
-  <si>
-    <t>DistributionLine</t>
-  </si>
-  <si>
-    <t>ElectricCarCharger</t>
-  </si>
-  <si>
-    <t>complete</t>
-  </si>
-  <si>
-    <t>addition</t>
-  </si>
-  <si>
-    <t>power</t>
-  </si>
-  <si>
-    <t>https://purl.orgl/neat/power/</t>
-  </si>
-  <si>
     <t>Power to Consumer Data Model</t>
   </si>
   <si>
@@ -396,18 +561,48 @@
     <t>http://purl.org/cognite/power_analytic</t>
   </si>
   <si>
+    <t>Power Forecast Model</t>
+  </si>
+  <si>
+    <t>Solution model for WindFarm power production forecast</t>
+  </si>
+  <si>
     <t>Olav</t>
   </si>
   <si>
-    <t>Power Forecast Model</t>
-  </si>
-  <si>
-    <t>Solution model for WindFarm power production forecast</t>
-  </si>
-  <si>
     <t>WeatherStation</t>
   </si>
   <si>
+    <t>PowerForecast</t>
+  </si>
+  <si>
+    <t>powerForecasts</t>
+  </si>
+  <si>
+    <t>minPowerForecast</t>
+  </si>
+  <si>
+    <t>mediumPowerForecast</t>
+  </si>
+  <si>
+    <t>maxPowerForecast</t>
+  </si>
+  <si>
+    <t>weatherForecasts</t>
+  </si>
+  <si>
+    <t>weatherObservations</t>
+  </si>
+  <si>
+    <t>lowPowerForecast</t>
+  </si>
+  <si>
+    <t>highPowerForecast</t>
+  </si>
+  <si>
+    <t>expectedPowerForecast</t>
+  </si>
+  <si>
     <t>source</t>
   </si>
   <si>
@@ -432,15 +627,6 @@
     <t>cloudAreaFraction</t>
   </si>
   <si>
-    <t>weatherForecasts</t>
-  </si>
-  <si>
-    <t>weatherObservations</t>
-  </si>
-  <si>
-    <t>PowerForecast</t>
-  </si>
-  <si>
     <t>algorithm</t>
   </si>
   <si>
@@ -450,37 +636,10 @@
     <t>parameters</t>
   </si>
   <si>
+    <t>json</t>
+  </si>
+  <si>
     <t>forecast</t>
-  </si>
-  <si>
-    <t>json</t>
-  </si>
-  <si>
-    <t>powerForecasts</t>
-  </si>
-  <si>
-    <t>minPowerForecast</t>
-  </si>
-  <si>
-    <t>mediumPowerForecast</t>
-  </si>
-  <si>
-    <t>maxPowerForecast</t>
-  </si>
-  <si>
-    <t>lowPowerForecast</t>
-  </si>
-  <si>
-    <t>highPowerForecast</t>
-  </si>
-  <si>
-    <t>expectedPowerForecast</t>
-  </si>
-  <si>
-    <t>power:WindFarm</t>
-  </si>
-  <si>
-    <t>power:GeoLocation</t>
   </si>
 </sst>
 </file>
@@ -502,19 +661,16 @@
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="20"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -894,17 +1050,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA13" sqref="AA13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="48.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -912,86 +1068,86 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="B4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="B5" s="6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="B6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="B7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="B8" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="B9" s="7">
         <v>45377</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="7">
         <v>45331</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>119</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{7A17D660-CDA8-4F5F-9BE5-36077EFE12B0}"/>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{96D942D6-E3E9-43DE-9C6E-39143A393B0B}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -999,25 +1155,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M47"/>
+  <dimension ref="A1:M40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.5" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.44140625" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="13" width="13" customWidth="1"/>
+    <col min="5" max="5" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="13" customWidth="1"/>
+    <col min="9" max="9" width="49.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -1032,84 +1190,90 @@
       <c r="L1" s="9"/>
       <c r="M1" s="9"/>
     </row>
-    <row r="2" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
         <v>29</v>
       </c>
-      <c r="E3" t="s">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
         <v>30</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
         <v>31</v>
       </c>
-      <c r="E4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
@@ -1123,33 +1287,39 @@
       <c r="G5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
         <v>36</v>
       </c>
-      <c r="B6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" t="s">
-        <v>35</v>
-      </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -1157,33 +1327,39 @@
       <c r="G7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="I8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>38</v>
       </c>
-      <c r="E8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>36</v>
-      </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -1191,16 +1367,19 @@
       <c r="G9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E10" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -1208,27 +1387,30 @@
       <c r="G10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>139</v>
+        <v>183</v>
       </c>
       <c r="E11" t="s">
-        <v>133</v>
+        <v>182</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>140</v>
+        <v>184</v>
       </c>
       <c r="E12" t="s">
         <v>33</v>
@@ -1240,12 +1422,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
-        <v>141</v>
+        <v>185</v>
       </c>
       <c r="E13" t="s">
         <v>33</v>
@@ -1257,12 +1439,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>142</v>
+        <v>186</v>
       </c>
       <c r="E14" t="s">
         <v>33</v>
@@ -1274,15 +1456,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="E16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -1290,16 +1472,19 @@
       <c r="G16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E17" t="s">
-        <v>90</v>
+        <v>129</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -1307,55 +1492,61 @@
       <c r="G17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E18" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="B19" t="s">
-        <v>131</v>
+        <v>187</v>
       </c>
       <c r="E19" t="s">
-        <v>122</v>
+        <v>181</v>
       </c>
       <c r="F19">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="B20" t="s">
-        <v>132</v>
+        <v>188</v>
       </c>
       <c r="E20" t="s">
-        <v>122</v>
+        <v>181</v>
       </c>
       <c r="F20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="B21" t="s">
-        <v>143</v>
+        <v>189</v>
       </c>
       <c r="E21" t="s">
         <v>33</v>
@@ -1367,12 +1558,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="B22" t="s">
-        <v>144</v>
+        <v>190</v>
       </c>
       <c r="E22" t="s">
         <v>33</v>
@@ -1384,12 +1575,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="B23" t="s">
-        <v>145</v>
+        <v>191</v>
       </c>
       <c r="E23" t="s">
         <v>33</v>
@@ -1401,32 +1592,49 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>84</v>
+        <v>181</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="E25" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>181</v>
+      </c>
+      <c r="B26" t="s">
         <v>30</v>
       </c>
-      <c r="F25">
-        <v>1</v>
-      </c>
-      <c r="G25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E26" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>85</v>
+        <v>181</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
+        <v>192</v>
       </c>
       <c r="E27" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -1435,15 +1643,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>85</v>
+        <v>181</v>
       </c>
       <c r="B28" t="s">
-        <v>87</v>
+        <v>193</v>
       </c>
       <c r="E28" t="s">
-        <v>39</v>
+        <v>121</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -1452,114 +1660,134 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>181</v>
+      </c>
+      <c r="B29" t="s">
+        <v>194</v>
+      </c>
+      <c r="E29" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>90</v>
+        <v>181</v>
       </c>
       <c r="B30" t="s">
-        <v>89</v>
+        <v>195</v>
       </c>
       <c r="E30" t="s">
-        <v>85</v>
+        <v>33</v>
       </c>
       <c r="F30">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>181</v>
+      </c>
+      <c r="B31" t="s">
+        <v>196</v>
+      </c>
+      <c r="E31" t="s">
+        <v>33</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>122</v>
+        <v>181</v>
       </c>
       <c r="B32" t="s">
-        <v>29</v>
+        <v>197</v>
       </c>
       <c r="E32" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G32">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>122</v>
+        <v>181</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>198</v>
       </c>
       <c r="E33" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G33">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>122</v>
+        <v>181</v>
       </c>
       <c r="B34" t="s">
-        <v>123</v>
+        <v>199</v>
       </c>
       <c r="E34" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G34">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>122</v>
-      </c>
-      <c r="B35" t="s">
-        <v>124</v>
-      </c>
-      <c r="E35" t="s">
-        <v>85</v>
-      </c>
-      <c r="F35">
-        <v>1</v>
-      </c>
-      <c r="G35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>122</v>
+        <v>182</v>
       </c>
       <c r="B36" t="s">
-        <v>125</v>
+        <v>5</v>
       </c>
       <c r="E36" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G36">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>122</v>
+        <v>182</v>
       </c>
       <c r="B37" t="s">
-        <v>126</v>
+        <v>200</v>
       </c>
       <c r="E37" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -1568,12 +1796,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>122</v>
+        <v>182</v>
       </c>
       <c r="B38" t="s">
-        <v>127</v>
+        <v>201</v>
       </c>
       <c r="E38" t="s">
         <v>33</v>
@@ -1581,19 +1809,16 @@
       <c r="F38">
         <v>0</v>
       </c>
-      <c r="G38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>122</v>
+        <v>182</v>
       </c>
       <c r="B39" t="s">
-        <v>128</v>
+        <v>202</v>
       </c>
       <c r="E39" t="s">
-        <v>33</v>
+        <v>203</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -1602,119 +1827,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>122</v>
+        <v>182</v>
       </c>
       <c r="B40" t="s">
-        <v>129</v>
+        <v>204</v>
       </c>
       <c r="E40" t="s">
         <v>33</v>
       </c>
       <c r="F40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>122</v>
-      </c>
-      <c r="B41" t="s">
-        <v>130</v>
-      </c>
-      <c r="E41" t="s">
-        <v>33</v>
-      </c>
-      <c r="F41">
-        <v>0</v>
-      </c>
-      <c r="G41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>133</v>
-      </c>
-      <c r="B43" t="s">
-        <v>29</v>
-      </c>
-      <c r="E43" t="s">
-        <v>30</v>
-      </c>
-      <c r="F43">
-        <v>1</v>
-      </c>
-      <c r="G43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>133</v>
-      </c>
-      <c r="B44" t="s">
-        <v>134</v>
-      </c>
-      <c r="E44" t="s">
-        <v>30</v>
-      </c>
-      <c r="F44">
-        <v>0</v>
-      </c>
-      <c r="G44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>133</v>
-      </c>
-      <c r="B45" t="s">
-        <v>135</v>
-      </c>
-      <c r="E45" t="s">
-        <v>33</v>
-      </c>
-      <c r="F45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>133</v>
-      </c>
-      <c r="B46" t="s">
-        <v>136</v>
-      </c>
-      <c r="E46" t="s">
-        <v>138</v>
-      </c>
-      <c r="F46">
-        <v>0</v>
-      </c>
-      <c r="G46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>133</v>
-      </c>
-      <c r="B47" t="s">
-        <v>137</v>
-      </c>
-      <c r="E47" t="s">
-        <v>33</v>
-      </c>
-      <c r="F47">
-        <v>1</v>
-      </c>
-      <c r="G47">
         <v>1</v>
       </c>
     </row>
@@ -1723,7 +1849,6 @@
     <mergeCell ref="A1:M1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1733,21 +1858,18 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F54" sqref="F54"/>
+      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" customWidth="1"/>
-    <col min="3" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13" customWidth="1"/>
+    <col min="1" max="1" width="21.44140625" customWidth="1"/>
+    <col min="2" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -1756,77 +1878,77 @@
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
     </row>
-    <row r="2" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="E2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="G2" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E4" t="s">
         <v>36</v>
       </c>
-      <c r="E3" t="s">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>90</v>
-      </c>
-      <c r="B7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>133</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -1842,24 +1964,24 @@
   <dimension ref="A1:M66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D55" sqref="D55"/>
+      <pane ySplit="2" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:M66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.5" customWidth="1"/>
-    <col min="2" max="2" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="34.44140625" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" customWidth="1"/>
     <col min="3" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="24.5" customWidth="1"/>
+    <col min="5" max="5" width="24.44140625" customWidth="1"/>
     <col min="6" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="40.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="53.44140625" customWidth="1"/>
     <col min="10" max="13" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -1874,58 +1996,58 @@
       <c r="L1" s="9"/>
       <c r="M1" s="9"/>
     </row>
-    <row r="2" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F3" s="3">
         <v>1</v>
@@ -1934,26 +2056,25 @@
         <v>1</v>
       </c>
       <c r="H3" s="3"/>
-      <c r="I3" s="3" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A3 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B3 &amp; ")"</f>
-        <v>power:GeneratingUnit(power:name)</v>
+      <c r="I3" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F4" s="3">
         <v>1</v>
@@ -1962,18 +2083,17 @@
         <v>1</v>
       </c>
       <c r="H4" s="3"/>
-      <c r="I4" s="3" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A4 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B4 &amp; ")"</f>
-        <v>power:GeneratingUnit(power:type)</v>
+      <c r="I4" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>32</v>
@@ -1990,26 +2110,25 @@
         <v>1</v>
       </c>
       <c r="H5" s="3"/>
-      <c r="I5" s="3" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A5 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B5 &amp; ")"</f>
-        <v>power:GeneratingUnit(power:activePower)</v>
+      <c r="I5" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F6" s="3">
         <v>0</v>
@@ -2018,16 +2137,15 @@
         <v>1</v>
       </c>
       <c r="H6" s="3"/>
-      <c r="I6" s="3" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A6 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B6 &amp; ")"</f>
-        <v>power:GeneratingUnit(power:geoLocation)</v>
+      <c r="I6" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -2042,17 +2160,17 @@
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F8" s="4">
         <v>0</v>
@@ -2061,26 +2179,25 @@
         <v>1</v>
       </c>
       <c r="H8" s="4"/>
-      <c r="I8" s="4" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A8 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B8 &amp; ")"</f>
-        <v>power:WindTurbine(power:manufacturer)</v>
+      <c r="I8" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F9" s="4">
         <v>1</v>
@@ -2089,26 +2206,25 @@
         <v>1</v>
       </c>
       <c r="H9" s="4"/>
-      <c r="I9" s="4" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A9 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B9 &amp; ")"</f>
-        <v>power:WindTurbine(power:ratedPower)</v>
+      <c r="I9" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F10" s="4">
         <v>1</v>
@@ -2117,26 +2233,25 @@
         <v>1</v>
       </c>
       <c r="H10" s="4"/>
-      <c r="I10" s="4" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A10 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B10 &amp; ")"</f>
-        <v>power:WindTurbine(power:hubHeight)</v>
+      <c r="I10" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F11" s="4">
         <v>0</v>
@@ -2145,26 +2260,25 @@
         <v>1</v>
       </c>
       <c r="H11" s="4"/>
-      <c r="I11" s="4" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A11 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B11 &amp; ")"</f>
-        <v>power:WindTurbine(power:arrayCableConnection)</v>
+      <c r="I11" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F12" s="4">
         <v>0</v>
@@ -2173,16 +2287,15 @@
         <v>1</v>
       </c>
       <c r="H12" s="4"/>
-      <c r="I12" s="4" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A12 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B12 &amp; ")"</f>
-        <v>power:WindTurbine(power:lifeExpectancy)</v>
+      <c r="I12" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -2197,17 +2310,17 @@
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F14" s="3">
         <v>1</v>
@@ -2216,26 +2329,25 @@
         <v>1</v>
       </c>
       <c r="H14" s="3"/>
-      <c r="I14" s="3" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A14 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B14 &amp; ")"</f>
-        <v>power:EnergyArea(power:name)</v>
+      <c r="I14" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="F15" s="3">
         <v>0</v>
@@ -2244,26 +2356,25 @@
         <v>1</v>
       </c>
       <c r="H15" s="3"/>
-      <c r="I15" s="3" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A15 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B15 &amp; ")"</f>
-        <v>power:EnergyArea(power:geoLocation)</v>
+      <c r="I15" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F16" s="3">
         <v>1</v>
@@ -2272,18 +2383,17 @@
         <v>1</v>
       </c>
       <c r="H16" s="3"/>
-      <c r="I16" s="3" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A16 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B16 &amp; ")"</f>
-        <v>power:EnergyArea(power:ratedPower)</v>
+      <c r="I16" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>32</v>
@@ -2300,16 +2410,15 @@
         <v>1</v>
       </c>
       <c r="H17" s="3"/>
-      <c r="I17" s="3" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A17 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B17 &amp; ")"</f>
-        <v>power:EnergyArea(power:activePower)</v>
+      <c r="I17" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -2324,17 +2433,17 @@
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="F19" s="4">
         <v>0</v>
@@ -2343,26 +2452,25 @@
         <v>1</v>
       </c>
       <c r="H19" s="4"/>
-      <c r="I19" s="4" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A19 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B19 &amp; ")"</f>
-        <v>power:WindFarm(power:substation)</v>
+      <c r="I19" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="F20" s="4">
         <v>0</v>
@@ -2371,68 +2479,65 @@
         <v>1</v>
       </c>
       <c r="H20" s="4"/>
-      <c r="I20" s="4" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A20 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B20 &amp; ")"</f>
-        <v>power:WindFarm(power:exportCable)</v>
+      <c r="I20" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F21" s="4">
         <v>0</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
-      <c r="I21" s="4" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A21 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B21 &amp; ")"</f>
-        <v>power:WindFarm(power:arrayCable)</v>
+      <c r="I21" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="F22" s="4">
         <v>0</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
-      <c r="I22" s="4" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A22 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B22 &amp; ")"</f>
-        <v>power:WindFarm(power:windTurbines)</v>
+      <c r="I22" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -2447,17 +2552,17 @@
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F24" s="3">
         <v>1</v>
@@ -2466,26 +2571,25 @@
         <v>1</v>
       </c>
       <c r="H24" s="3"/>
-      <c r="I24" s="3" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A24 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B24 &amp; ")"</f>
-        <v>power:Substation(power:name)</v>
+      <c r="I24" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F25" s="3">
         <v>0</v>
@@ -2494,26 +2598,25 @@
         <v>1</v>
       </c>
       <c r="H25" s="3"/>
-      <c r="I25" s="3" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A25 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B25 &amp; ")"</f>
-        <v>power:Substation(power:location)</v>
+      <c r="I25" s="3" t="s">
+        <v>73</v>
       </c>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="F26" s="3">
         <v>0</v>
@@ -2522,26 +2625,25 @@
         <v>1</v>
       </c>
       <c r="H26" s="3"/>
-      <c r="I26" s="3" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A26 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B26 &amp; ")"</f>
-        <v>power:Substation(power:mainTransformer)</v>
+      <c r="I26" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="F27" s="3">
         <v>0</v>
@@ -2550,26 +2652,25 @@
         <v>1</v>
       </c>
       <c r="H27" s="3"/>
-      <c r="I27" s="3" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A27 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B27 &amp; ")"</f>
-        <v>power:Substation(power:primaryPowerLine)</v>
+      <c r="I27" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="F28" s="3">
         <v>0</v>
@@ -2578,21 +2679,20 @@
         <v>1</v>
       </c>
       <c r="H28" s="3"/>
-      <c r="I28" s="3" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A28 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B28 &amp; ")"</f>
-        <v>power:Substation(power:secondaryPowerLine)</v>
+      <c r="I28" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -2606,21 +2706,20 @@
         <v>1</v>
       </c>
       <c r="H29" s="3"/>
-      <c r="I29" s="3" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A29 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B29 &amp; ")"</f>
-        <v>power:Substation(power:primaryVoltage)</v>
+      <c r="I29" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -2634,94 +2733,90 @@
         <v>1</v>
       </c>
       <c r="H30" s="3"/>
-      <c r="I30" s="3" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A30 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B30 &amp; ")"</f>
-        <v>power:Substation(power:secondaryVoltage)</v>
+      <c r="I30" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="F31" s="3">
         <v>0</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
-      <c r="I31" s="3" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A31 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B31 &amp; ")"</f>
-        <v>power:Substation(power:circuitBreaker)</v>
+      <c r="I31" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="F32" s="3">
         <v>0</v>
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
-      <c r="I32" s="3" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A32 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B32 &amp; ")"</f>
-        <v>power:Substation(power:disconnectSwitch)</v>
+      <c r="I32" s="3" t="s">
+        <v>91</v>
       </c>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="F33" s="3">
         <v>0</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
-      <c r="I33" s="3" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefProperties!A33 &amp; "(" &amp; RefMetadata!B4&amp; ":" &amp;RefProperties!B33 &amp; ")"</f>
-        <v>power:Substation(power:currentTransformer)</v>
+      <c r="I33" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -2736,17 +2831,17 @@
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="F35" s="4">
         <v>0</v>
@@ -2755,23 +2850,25 @@
         <v>1</v>
       </c>
       <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
+      <c r="I35" s="4" t="s">
+        <v>98</v>
+      </c>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="F36" s="4">
         <v>0</v>
@@ -2780,18 +2877,20 @@
         <v>1</v>
       </c>
       <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
+      <c r="I36" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
@@ -2805,23 +2904,25 @@
         <v>1</v>
       </c>
       <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
+      <c r="I37" s="4" t="s">
+        <v>102</v>
+      </c>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>75</v>
+        <v>103</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F38" s="4">
         <v>0</v>
@@ -2830,13 +2931,15 @@
         <v>1</v>
       </c>
       <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
+      <c r="I38" s="4" t="s">
+        <v>104</v>
+      </c>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -2851,17 +2954,17 @@
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3" t="s">
-        <v>78</v>
+        <v>107</v>
       </c>
       <c r="F40" s="3">
         <v>0</v>
@@ -2870,18 +2973,20 @@
         <v>1</v>
       </c>
       <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
+      <c r="I40" s="3" t="s">
+        <v>108</v>
+      </c>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>79</v>
+        <v>109</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
@@ -2895,36 +3000,40 @@
         <v>1</v>
       </c>
       <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
+      <c r="I41" s="3" t="s">
+        <v>110</v>
+      </c>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>80</v>
+        <v>111</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3" t="s">
-        <v>81</v>
+        <v>112</v>
       </c>
       <c r="F42" s="3">
         <v>0</v>
       </c>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
+      <c r="I42" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -2939,17 +3048,17 @@
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>82</v>
+        <v>114</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F44" s="4">
         <v>1</v>
@@ -2958,23 +3067,25 @@
         <v>1</v>
       </c>
       <c r="H44" s="4"/>
-      <c r="I44" s="4"/>
+      <c r="I44" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
       <c r="M44" s="4"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
-        <v>82</v>
+        <v>114</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F45" s="4">
         <v>0</v>
@@ -2983,18 +3094,20 @@
         <v>1</v>
       </c>
       <c r="H45" s="4"/>
-      <c r="I45" s="4"/>
+      <c r="I45" s="4" t="s">
+        <v>116</v>
+      </c>
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
       <c r="L45" s="4"/>
       <c r="M45" s="4"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
-        <v>82</v>
+        <v>114</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>83</v>
+        <v>117</v>
       </c>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
@@ -3008,13 +3121,15 @@
         <v>1</v>
       </c>
       <c r="H46" s="4"/>
-      <c r="I46" s="4"/>
+      <c r="I46" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
       <c r="L46" s="4"/>
       <c r="M46" s="4"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -3029,17 +3144,17 @@
       <c r="L47" s="4"/>
       <c r="M47" s="4"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>84</v>
+        <v>119</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F48" s="3">
         <v>1</v>
@@ -3048,13 +3163,15 @@
         <v>1</v>
       </c>
       <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
+      <c r="I48" s="3" t="s">
+        <v>120</v>
+      </c>
       <c r="J48" s="3"/>
       <c r="K48" s="3"/>
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -3069,17 +3186,17 @@
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
-        <v>85</v>
+        <v>121</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>86</v>
+        <v>122</v>
       </c>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
       <c r="E50" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F50" s="4">
         <v>1</v>
@@ -3088,23 +3205,25 @@
         <v>1</v>
       </c>
       <c r="H50" s="4"/>
-      <c r="I50" s="4"/>
+      <c r="I50" s="4" t="s">
+        <v>123</v>
+      </c>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
-        <v>85</v>
+        <v>121</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>87</v>
+        <v>124</v>
       </c>
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
       <c r="E51" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F51" s="4">
         <v>1</v>
@@ -3113,13 +3232,15 @@
         <v>1</v>
       </c>
       <c r="H51" s="4"/>
-      <c r="I51" s="4"/>
+      <c r="I51" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -3134,30 +3255,32 @@
       <c r="L52" s="4"/>
       <c r="M52" s="4"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>88</v>
+        <v>126</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>89</v>
+        <v>127</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
       <c r="E53" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F53" s="3">
         <v>0</v>
       </c>
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
-      <c r="I53" s="3"/>
+      <c r="I53" s="3" t="s">
+        <v>128</v>
+      </c>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
       <c r="L53" s="3"/>
       <c r="M53" s="3"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -3172,30 +3295,32 @@
       <c r="L54" s="3"/>
       <c r="M54" s="3"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
-        <v>90</v>
+        <v>129</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>89</v>
+        <v>127</v>
       </c>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
       <c r="E55" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F55" s="4">
         <v>0</v>
       </c>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
-      <c r="I55" s="4"/>
+      <c r="I55" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -3210,17 +3335,17 @@
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>92</v>
+        <v>132</v>
       </c>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
       <c r="E57" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F57" s="3">
         <v>0</v>
@@ -3229,13 +3354,15 @@
         <v>1</v>
       </c>
       <c r="H57" s="3"/>
-      <c r="I57" s="3"/>
+      <c r="I57" s="3" t="s">
+        <v>133</v>
+      </c>
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
       <c r="L57" s="3"/>
       <c r="M57" s="3"/>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -3250,17 +3377,17 @@
       <c r="L58" s="3"/>
       <c r="M58" s="3"/>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
-        <v>93</v>
+        <v>134</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>92</v>
+        <v>132</v>
       </c>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
       <c r="E59" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F59" s="4">
         <v>0</v>
@@ -3269,13 +3396,15 @@
         <v>1</v>
       </c>
       <c r="H59" s="4"/>
-      <c r="I59" s="4"/>
+      <c r="I59" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
       <c r="L59" s="4"/>
       <c r="M59" s="4"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -3290,17 +3419,17 @@
       <c r="L60" s="4"/>
       <c r="M60" s="4"/>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
-        <v>94</v>
+        <v>136</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>92</v>
+        <v>132</v>
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
       <c r="E61" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F61" s="3">
         <v>0</v>
@@ -3309,13 +3438,15 @@
         <v>1</v>
       </c>
       <c r="H61" s="3"/>
-      <c r="I61" s="3"/>
+      <c r="I61" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="J61" s="3"/>
       <c r="K61" s="3"/>
       <c r="L61" s="3"/>
       <c r="M61" s="3"/>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -3330,17 +3461,17 @@
       <c r="L62" s="3"/>
       <c r="M62" s="3"/>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
-        <v>95</v>
+        <v>138</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>96</v>
+        <v>139</v>
       </c>
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
       <c r="E63" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F63" s="4">
         <v>1</v>
@@ -3349,13 +3480,15 @@
         <v>1</v>
       </c>
       <c r="H63" s="4"/>
-      <c r="I63" s="4"/>
+      <c r="I63" s="4" t="s">
+        <v>140</v>
+      </c>
       <c r="J63" s="4"/>
       <c r="K63" s="4"/>
       <c r="L63" s="4"/>
       <c r="M63" s="4"/>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
@@ -3370,17 +3503,17 @@
       <c r="L64" s="4"/>
       <c r="M64" s="4"/>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
-        <v>97</v>
+        <v>141</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>98</v>
+        <v>142</v>
       </c>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
       <c r="E65" s="3" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="F65" s="3">
         <v>0</v>
@@ -3389,23 +3522,25 @@
         <v>1</v>
       </c>
       <c r="H65" s="3"/>
-      <c r="I65" s="3"/>
+      <c r="I65" s="3" t="s">
+        <v>143</v>
+      </c>
       <c r="J65" s="3"/>
       <c r="K65" s="3"/>
       <c r="L65" s="3"/>
       <c r="M65" s="3"/>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
-        <v>97</v>
+        <v>141</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>99</v>
+        <v>144</v>
       </c>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
       <c r="E66" s="3" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="F66" s="3">
         <v>0</v>
@@ -3414,7 +3549,9 @@
         <v>1</v>
       </c>
       <c r="H66" s="3"/>
-      <c r="I66" s="3"/>
+      <c r="I66" s="3" t="s">
+        <v>145</v>
+      </c>
       <c r="J66" s="3"/>
       <c r="K66" s="3"/>
       <c r="L66" s="3"/>
@@ -3425,7 +3562,6 @@
     <mergeCell ref="A1:M1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -3433,22 +3569,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="22.5" customWidth="1"/>
+    <col min="1" max="2" width="22.44140625" customWidth="1"/>
     <col min="3" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="24.33203125" customWidth="1"/>
+    <col min="5" max="5" width="28.44140625" customWidth="1"/>
     <col min="6" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -3457,303 +3593,277 @@
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
     </row>
-    <row r="2" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A3</f>
-        <v>power:GeneratingUnit</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>151</v>
+      </c>
+      <c r="B9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>153</v>
+      </c>
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>155</v>
+      </c>
+      <c r="B11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>157</v>
+      </c>
+      <c r="B13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>158</v>
+      </c>
+      <c r="B14" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>159</v>
+      </c>
+      <c r="B15" t="s">
+        <v>95</v>
+      </c>
+      <c r="E15" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>161</v>
+      </c>
+      <c r="B16" t="s">
+        <v>95</v>
+      </c>
+      <c r="E16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>105</v>
+      </c>
+      <c r="E17" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>114</v>
+      </c>
+      <c r="E18" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>164</v>
+      </c>
+      <c r="B19" t="s">
+        <v>114</v>
+      </c>
+      <c r="E19" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>119</v>
+      </c>
+      <c r="E20" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>121</v>
+      </c>
+      <c r="B21" t="s">
+        <v>119</v>
+      </c>
+      <c r="E21" t="s">
         <v>36</v>
       </c>
-      <c r="B4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A4</f>
-        <v>power:WindTurbine</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E5" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A5</f>
-        <v>power:EnergyArea</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A6</f>
-        <v>power:WindFarm</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>55</v>
-      </c>
-      <c r="E7" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A7</f>
-        <v>power:Substation</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>100</v>
-      </c>
-      <c r="B8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E8" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A8</f>
-        <v>power:OffshoreSubstation</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>101</v>
-      </c>
-      <c r="B9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A9</f>
-        <v>power:TransmissionSubstation</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>102</v>
-      </c>
-      <c r="B10" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A10</f>
-        <v>power:DistributionSubstation</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>103</v>
-      </c>
-      <c r="B11" t="s">
-        <v>101</v>
-      </c>
-      <c r="E11" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A11</f>
-        <v>power:OnshoreSubstation</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E12" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A12</f>
-        <v>power:PowerLine</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>104</v>
-      </c>
-      <c r="B13" t="s">
-        <v>70</v>
-      </c>
-      <c r="E13" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A13</f>
-        <v>power:ArrayCable</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>105</v>
-      </c>
-      <c r="B14" t="s">
-        <v>70</v>
-      </c>
-      <c r="E14" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A14</f>
-        <v>power:ExportCable</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>106</v>
-      </c>
-      <c r="B15" t="s">
-        <v>70</v>
-      </c>
-      <c r="E15" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A15</f>
-        <v>power:Transmission</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>107</v>
-      </c>
-      <c r="B16" t="s">
-        <v>70</v>
-      </c>
-      <c r="E16" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A16</f>
-        <v>power:DistributionLine</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>76</v>
-      </c>
-      <c r="E17" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A17</f>
-        <v>power:Meter</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>82</v>
-      </c>
-      <c r="E18" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A18</f>
-        <v>power:EnergyConsumer</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>108</v>
-      </c>
-      <c r="B19" t="s">
-        <v>82</v>
-      </c>
-      <c r="E19" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A19</f>
-        <v>power:ElectricCarCharger</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>84</v>
-      </c>
-      <c r="E20" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A20</f>
-        <v>power:GeoLocation</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>85</v>
-      </c>
-      <c r="B21" t="s">
-        <v>84</v>
-      </c>
-      <c r="E21" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A21</f>
-        <v>power:Point</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>88</v>
+        <v>126</v>
       </c>
       <c r="B22" t="s">
-        <v>84</v>
-      </c>
-      <c r="E22" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A22</f>
-        <v>power:MultiLineString</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+      <c r="E22" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>129</v>
+      </c>
+      <c r="B23" t="s">
+        <v>119</v>
+      </c>
+      <c r="E23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>131</v>
+      </c>
+      <c r="E24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>134</v>
+      </c>
+      <c r="E25" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>136</v>
+      </c>
+      <c r="E26" t="s">
         <v>90</v>
       </c>
-      <c r="B23" t="s">
-        <v>84</v>
-      </c>
-      <c r="E23" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A23</f>
-        <v>power:Polygon</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>91</v>
-      </c>
-      <c r="E24" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A24</f>
-        <v>power:CircuitBreaker</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>93</v>
-      </c>
-      <c r="E25" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A25</f>
-        <v>power:CurrentTransformer</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>94</v>
-      </c>
-      <c r="E26" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A26</f>
-        <v>power:DisconnectSwitch</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>95</v>
-      </c>
-      <c r="E27" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A27</f>
-        <v>power:VoltageLevel</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+      <c r="E27" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>97</v>
-      </c>
-      <c r="E28" t="str">
-        <f>RefMetadata!B4&amp; ":" &amp;RefClasses!A28</f>
-        <v>power:VoltageTransformer</v>
+        <v>141</v>
+      </c>
+      <c r="E28" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -3768,17 +3878,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="29.5" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3786,81 +3894,81 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="B3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="B4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="B5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+    </row>
+    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="B8" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="B9" s="5">
+        <v>45388.62510806237</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="5">
-        <v>45377.41672594368</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="B10" s="5">
+        <v>45388.62510806237</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="5">
-        <v>45377.41672594368</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="B11" t="s">
-        <v>115</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: added dataModelType to information sheets
</commit_message>
<xml_diff>
--- a/docs/artifacts/rules/information-analytics-olav.xlsx
+++ b/docs/artifacts/rules/information-analytics-olav.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\artifacts\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A313EF-B9A8-4346-9BDE-7862A36F3900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43ADF53B-74A3-4BBF-AC84-362A31C96FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="207">
   <si>
     <t>role</t>
   </si>
@@ -640,6 +640,12 @@
   </si>
   <si>
     <t>forecast</t>
+  </si>
+  <si>
+    <t>dataModelType</t>
+  </si>
+  <si>
+    <t>solution</t>
   </si>
 </sst>
 </file>
@@ -1048,19 +1054,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA13" sqref="AA13"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="48.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1068,7 +1074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>166</v>
       </c>
@@ -1076,78 +1082,86 @@
         <v>175</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B6" s="6" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B10" s="7">
         <v>45377</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B11" s="7">
         <v>45331</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>180</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{96D942D6-E3E9-43DE-9C6E-39143A393B0B}"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{96D942D6-E3E9-43DE-9C6E-39143A393B0B}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1162,18 +1176,18 @@
       <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="49.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="49.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="13" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:13" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
         <v>11</v>
       </c>
@@ -1190,7 +1204,7 @@
       <c r="L1" s="9"/>
       <c r="M1" s="9"/>
     </row>
-    <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -1231,7 +1245,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -1251,7 +1265,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1271,7 +1285,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -1291,7 +1305,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -1311,7 +1325,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -1331,7 +1345,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1351,7 +1365,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -1371,7 +1385,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -1391,7 +1405,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -1405,7 +1419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -1422,7 +1436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -1439,7 +1453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -1456,7 +1470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>58</v>
       </c>
@@ -1476,7 +1490,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>58</v>
       </c>
@@ -1496,7 +1510,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -1513,7 +1527,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>58</v>
       </c>
@@ -1527,7 +1541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>58</v>
       </c>
@@ -1541,7 +1555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>58</v>
       </c>
@@ -1558,7 +1572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>58</v>
       </c>
@@ -1575,7 +1589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>58</v>
       </c>
@@ -1592,7 +1606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>181</v>
       </c>
@@ -1609,7 +1623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>181</v>
       </c>
@@ -1626,7 +1640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>181</v>
       </c>
@@ -1643,7 +1657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>181</v>
       </c>
@@ -1660,7 +1674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>181</v>
       </c>
@@ -1677,7 +1691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>181</v>
       </c>
@@ -1694,7 +1708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>181</v>
       </c>
@@ -1711,7 +1725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>181</v>
       </c>
@@ -1728,7 +1742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>181</v>
       </c>
@@ -1745,7 +1759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>181</v>
       </c>
@@ -1762,7 +1776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>182</v>
       </c>
@@ -1779,7 +1793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>182</v>
       </c>
@@ -1796,7 +1810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>182</v>
       </c>
@@ -1810,7 +1824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>182</v>
       </c>
@@ -1827,7 +1841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>182</v>
       </c>
@@ -1861,13 +1875,13 @@
       <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.44140625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
     <col min="2" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
         <v>25</v>
       </c>
@@ -1878,7 +1892,7 @@
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
     </row>
-    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -1901,7 +1915,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>119</v>
       </c>
@@ -1909,7 +1923,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>121</v>
       </c>
@@ -1920,7 +1934,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>129</v>
       </c>
@@ -1931,22 +1945,22 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>182</v>
       </c>
@@ -1968,18 +1982,18 @@
       <selection pane="bottomLeft" activeCell="A3" sqref="A3:M66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" customWidth="1"/>
-    <col min="2" max="2" width="20.44140625" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
     <col min="3" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="24.44140625" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" customWidth="1"/>
     <col min="6" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="53.44140625" customWidth="1"/>
+    <col min="9" max="9" width="53.42578125" customWidth="1"/>
     <col min="10" max="13" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:13" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
         <v>11</v>
       </c>
@@ -1996,7 +2010,7 @@
       <c r="L1" s="9"/>
       <c r="M1" s="9"/>
     </row>
-    <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -2037,7 +2051,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
@@ -2064,7 +2078,7 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>27</v>
       </c>
@@ -2091,7 +2105,7 @@
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
@@ -2118,7 +2132,7 @@
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>27</v>
       </c>
@@ -2145,7 +2159,7 @@
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -2160,7 +2174,7 @@
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>38</v>
       </c>
@@ -2187,7 +2201,7 @@
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>38</v>
       </c>
@@ -2214,7 +2228,7 @@
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>38</v>
       </c>
@@ -2241,7 +2255,7 @@
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>38</v>
       </c>
@@ -2268,7 +2282,7 @@
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>38</v>
       </c>
@@ -2295,7 +2309,7 @@
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -2310,7 +2324,7 @@
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>52</v>
       </c>
@@ -2337,7 +2351,7 @@
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>52</v>
       </c>
@@ -2364,7 +2378,7 @@
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>52</v>
       </c>
@@ -2391,7 +2405,7 @@
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>52</v>
       </c>
@@ -2418,7 +2432,7 @@
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -2433,7 +2447,7 @@
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>58</v>
       </c>
@@ -2460,7 +2474,7 @@
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>58</v>
       </c>
@@ -2487,7 +2501,7 @@
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>58</v>
       </c>
@@ -2512,7 +2526,7 @@
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>58</v>
       </c>
@@ -2537,7 +2551,7 @@
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -2552,7 +2566,7 @@
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>70</v>
       </c>
@@ -2579,7 +2593,7 @@
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>70</v>
       </c>
@@ -2606,7 +2620,7 @@
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>70</v>
       </c>
@@ -2633,7 +2647,7 @@
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>70</v>
       </c>
@@ -2660,7 +2674,7 @@
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>70</v>
       </c>
@@ -2687,7 +2701,7 @@
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>70</v>
       </c>
@@ -2714,7 +2728,7 @@
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>70</v>
       </c>
@@ -2741,7 +2755,7 @@
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>70</v>
       </c>
@@ -2766,7 +2780,7 @@
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>70</v>
       </c>
@@ -2791,7 +2805,7 @@
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>70</v>
       </c>
@@ -2816,7 +2830,7 @@
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -2831,7 +2845,7 @@
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>95</v>
       </c>
@@ -2858,7 +2872,7 @@
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>95</v>
       </c>
@@ -2885,7 +2899,7 @@
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>95</v>
       </c>
@@ -2912,7 +2926,7 @@
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>95</v>
       </c>
@@ -2939,7 +2953,7 @@
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -2954,7 +2968,7 @@
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>105</v>
       </c>
@@ -2981,7 +2995,7 @@
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>105</v>
       </c>
@@ -3008,7 +3022,7 @@
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>105</v>
       </c>
@@ -3033,7 +3047,7 @@
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -3048,7 +3062,7 @@
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>114</v>
       </c>
@@ -3075,7 +3089,7 @@
       <c r="L44" s="4"/>
       <c r="M44" s="4"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>114</v>
       </c>
@@ -3102,7 +3116,7 @@
       <c r="L45" s="4"/>
       <c r="M45" s="4"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>114</v>
       </c>
@@ -3129,7 +3143,7 @@
       <c r="L46" s="4"/>
       <c r="M46" s="4"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -3144,7 +3158,7 @@
       <c r="L47" s="4"/>
       <c r="M47" s="4"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>119</v>
       </c>
@@ -3171,7 +3185,7 @@
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -3186,7 +3200,7 @@
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>121</v>
       </c>
@@ -3213,7 +3227,7 @@
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>121</v>
       </c>
@@ -3240,7 +3254,7 @@
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -3255,7 +3269,7 @@
       <c r="L52" s="4"/>
       <c r="M52" s="4"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>126</v>
       </c>
@@ -3280,7 +3294,7 @@
       <c r="L53" s="3"/>
       <c r="M53" s="3"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -3295,7 +3309,7 @@
       <c r="L54" s="3"/>
       <c r="M54" s="3"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>129</v>
       </c>
@@ -3320,7 +3334,7 @@
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -3335,7 +3349,7 @@
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>131</v>
       </c>
@@ -3362,7 +3376,7 @@
       <c r="L57" s="3"/>
       <c r="M57" s="3"/>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -3377,7 +3391,7 @@
       <c r="L58" s="3"/>
       <c r="M58" s="3"/>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>134</v>
       </c>
@@ -3404,7 +3418,7 @@
       <c r="L59" s="4"/>
       <c r="M59" s="4"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -3419,7 +3433,7 @@
       <c r="L60" s="4"/>
       <c r="M60" s="4"/>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>136</v>
       </c>
@@ -3446,7 +3460,7 @@
       <c r="L61" s="3"/>
       <c r="M61" s="3"/>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -3461,7 +3475,7 @@
       <c r="L62" s="3"/>
       <c r="M62" s="3"/>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>138</v>
       </c>
@@ -3488,7 +3502,7 @@
       <c r="L63" s="4"/>
       <c r="M63" s="4"/>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
@@ -3503,7 +3517,7 @@
       <c r="L64" s="4"/>
       <c r="M64" s="4"/>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>141</v>
       </c>
@@ -3530,7 +3544,7 @@
       <c r="L65" s="3"/>
       <c r="M65" s="3"/>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>141</v>
       </c>
@@ -3574,15 +3588,15 @@
       <selection pane="bottomLeft" activeCell="A3" sqref="A3:E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="22.44140625" customWidth="1"/>
+    <col min="1" max="2" width="22.42578125" customWidth="1"/>
     <col min="3" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="28.44140625" customWidth="1"/>
+    <col min="5" max="5" width="28.42578125" customWidth="1"/>
     <col min="6" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
         <v>25</v>
       </c>
@@ -3593,7 +3607,7 @@
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
     </row>
-    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -3616,7 +3630,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -3624,7 +3638,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -3635,7 +3649,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -3643,7 +3657,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -3654,7 +3668,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>70</v>
       </c>
@@ -3662,7 +3676,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>150</v>
       </c>
@@ -3673,7 +3687,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>151</v>
       </c>
@@ -3684,7 +3698,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>153</v>
       </c>
@@ -3695,7 +3709,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>155</v>
       </c>
@@ -3706,7 +3720,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>95</v>
       </c>
@@ -3714,7 +3728,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>157</v>
       </c>
@@ -3725,7 +3739,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>158</v>
       </c>
@@ -3736,7 +3750,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>159</v>
       </c>
@@ -3747,7 +3761,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>161</v>
       </c>
@@ -3758,7 +3772,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>105</v>
       </c>
@@ -3766,7 +3780,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>114</v>
       </c>
@@ -3774,7 +3788,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>164</v>
       </c>
@@ -3785,7 +3799,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>119</v>
       </c>
@@ -3793,7 +3807,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>121</v>
       </c>
@@ -3804,7 +3818,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>126</v>
       </c>
@@ -3815,7 +3829,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>129</v>
       </c>
@@ -3826,7 +3840,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>131</v>
       </c>
@@ -3834,7 +3848,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>134</v>
       </c>
@@ -3842,7 +3856,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>136</v>
       </c>
@@ -3850,7 +3864,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>138</v>
       </c>
@@ -3858,7 +3872,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>141</v>
       </c>
@@ -3880,13 +3894,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="29.44140625" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3894,7 +3908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>166</v>
       </c>
@@ -3902,7 +3916,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -3910,7 +3924,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -3918,7 +3932,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -3926,7 +3940,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>171</v>
       </c>
@@ -3934,12 +3948,12 @@
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -3947,7 +3961,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -3955,7 +3969,7 @@
         <v>45388.62510806237</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -3963,7 +3977,7 @@
         <v>45388.62510806237</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
[NEAT-218] 🐻‍❄️ Ensure Lifecycle Tutorials are up-to-date (#457)
* refactor: Remove warning

* refactor: Update overview

* docs; Some extra newlines and fixes

* refactor: update

* refactor: added license and rights

* docs: updated David part

* docs: Update Alice

* docs: updated part 2

* docs Update part 3

* refactor: added dataModelType to information sheets

* refactor: Added ref model option for ExcelToRules

* refactor: added missing options for steps

* refactor: added missing modal

* docs: Finished part 3

* refactor: review feedback
</commit_message>
<xml_diff>
--- a/docs/artifacts/rules/information-analytics-olav.xlsx
+++ b/docs/artifacts/rules/information-analytics-olav.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\artifacts\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A313EF-B9A8-4346-9BDE-7862A36F3900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43ADF53B-74A3-4BBF-AC84-362A31C96FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="207">
   <si>
     <t>role</t>
   </si>
@@ -640,6 +640,12 @@
   </si>
   <si>
     <t>forecast</t>
+  </si>
+  <si>
+    <t>dataModelType</t>
+  </si>
+  <si>
+    <t>solution</t>
   </si>
 </sst>
 </file>
@@ -1048,19 +1054,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA13" sqref="AA13"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="48.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1068,7 +1074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>166</v>
       </c>
@@ -1076,78 +1082,86 @@
         <v>175</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B6" s="6" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B10" s="7">
         <v>45377</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B11" s="7">
         <v>45331</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>180</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{96D942D6-E3E9-43DE-9C6E-39143A393B0B}"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{96D942D6-E3E9-43DE-9C6E-39143A393B0B}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1162,18 +1176,18 @@
       <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="49.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="49.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="13" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:13" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
         <v>11</v>
       </c>
@@ -1190,7 +1204,7 @@
       <c r="L1" s="9"/>
       <c r="M1" s="9"/>
     </row>
-    <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -1231,7 +1245,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -1251,7 +1265,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1271,7 +1285,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -1291,7 +1305,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -1311,7 +1325,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -1331,7 +1345,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1351,7 +1365,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -1371,7 +1385,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -1391,7 +1405,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -1405,7 +1419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -1422,7 +1436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -1439,7 +1453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -1456,7 +1470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>58</v>
       </c>
@@ -1476,7 +1490,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>58</v>
       </c>
@@ -1496,7 +1510,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -1513,7 +1527,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>58</v>
       </c>
@@ -1527,7 +1541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>58</v>
       </c>
@@ -1541,7 +1555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>58</v>
       </c>
@@ -1558,7 +1572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>58</v>
       </c>
@@ -1575,7 +1589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>58</v>
       </c>
@@ -1592,7 +1606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>181</v>
       </c>
@@ -1609,7 +1623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>181</v>
       </c>
@@ -1626,7 +1640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>181</v>
       </c>
@@ -1643,7 +1657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>181</v>
       </c>
@@ -1660,7 +1674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>181</v>
       </c>
@@ -1677,7 +1691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>181</v>
       </c>
@@ -1694,7 +1708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>181</v>
       </c>
@@ -1711,7 +1725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>181</v>
       </c>
@@ -1728,7 +1742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>181</v>
       </c>
@@ -1745,7 +1759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>181</v>
       </c>
@@ -1762,7 +1776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>182</v>
       </c>
@@ -1779,7 +1793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>182</v>
       </c>
@@ -1796,7 +1810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>182</v>
       </c>
@@ -1810,7 +1824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>182</v>
       </c>
@@ -1827,7 +1841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>182</v>
       </c>
@@ -1861,13 +1875,13 @@
       <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.44140625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
     <col min="2" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
         <v>25</v>
       </c>
@@ -1878,7 +1892,7 @@
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
     </row>
-    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -1901,7 +1915,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>119</v>
       </c>
@@ -1909,7 +1923,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>121</v>
       </c>
@@ -1920,7 +1934,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>129</v>
       </c>
@@ -1931,22 +1945,22 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>182</v>
       </c>
@@ -1968,18 +1982,18 @@
       <selection pane="bottomLeft" activeCell="A3" sqref="A3:M66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" customWidth="1"/>
-    <col min="2" max="2" width="20.44140625" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
     <col min="3" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="24.44140625" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" customWidth="1"/>
     <col min="6" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="53.44140625" customWidth="1"/>
+    <col min="9" max="9" width="53.42578125" customWidth="1"/>
     <col min="10" max="13" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:13" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
         <v>11</v>
       </c>
@@ -1996,7 +2010,7 @@
       <c r="L1" s="9"/>
       <c r="M1" s="9"/>
     </row>
-    <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -2037,7 +2051,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
@@ -2064,7 +2078,7 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>27</v>
       </c>
@@ -2091,7 +2105,7 @@
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
@@ -2118,7 +2132,7 @@
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>27</v>
       </c>
@@ -2145,7 +2159,7 @@
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -2160,7 +2174,7 @@
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>38</v>
       </c>
@@ -2187,7 +2201,7 @@
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>38</v>
       </c>
@@ -2214,7 +2228,7 @@
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>38</v>
       </c>
@@ -2241,7 +2255,7 @@
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>38</v>
       </c>
@@ -2268,7 +2282,7 @@
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>38</v>
       </c>
@@ -2295,7 +2309,7 @@
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -2310,7 +2324,7 @@
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>52</v>
       </c>
@@ -2337,7 +2351,7 @@
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>52</v>
       </c>
@@ -2364,7 +2378,7 @@
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>52</v>
       </c>
@@ -2391,7 +2405,7 @@
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>52</v>
       </c>
@@ -2418,7 +2432,7 @@
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -2433,7 +2447,7 @@
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>58</v>
       </c>
@@ -2460,7 +2474,7 @@
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>58</v>
       </c>
@@ -2487,7 +2501,7 @@
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>58</v>
       </c>
@@ -2512,7 +2526,7 @@
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>58</v>
       </c>
@@ -2537,7 +2551,7 @@
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -2552,7 +2566,7 @@
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>70</v>
       </c>
@@ -2579,7 +2593,7 @@
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>70</v>
       </c>
@@ -2606,7 +2620,7 @@
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>70</v>
       </c>
@@ -2633,7 +2647,7 @@
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>70</v>
       </c>
@@ -2660,7 +2674,7 @@
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>70</v>
       </c>
@@ -2687,7 +2701,7 @@
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>70</v>
       </c>
@@ -2714,7 +2728,7 @@
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>70</v>
       </c>
@@ -2741,7 +2755,7 @@
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>70</v>
       </c>
@@ -2766,7 +2780,7 @@
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>70</v>
       </c>
@@ -2791,7 +2805,7 @@
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>70</v>
       </c>
@@ -2816,7 +2830,7 @@
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -2831,7 +2845,7 @@
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>95</v>
       </c>
@@ -2858,7 +2872,7 @@
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>95</v>
       </c>
@@ -2885,7 +2899,7 @@
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>95</v>
       </c>
@@ -2912,7 +2926,7 @@
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>95</v>
       </c>
@@ -2939,7 +2953,7 @@
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -2954,7 +2968,7 @@
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>105</v>
       </c>
@@ -2981,7 +2995,7 @@
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>105</v>
       </c>
@@ -3008,7 +3022,7 @@
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>105</v>
       </c>
@@ -3033,7 +3047,7 @@
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -3048,7 +3062,7 @@
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>114</v>
       </c>
@@ -3075,7 +3089,7 @@
       <c r="L44" s="4"/>
       <c r="M44" s="4"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>114</v>
       </c>
@@ -3102,7 +3116,7 @@
       <c r="L45" s="4"/>
       <c r="M45" s="4"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>114</v>
       </c>
@@ -3129,7 +3143,7 @@
       <c r="L46" s="4"/>
       <c r="M46" s="4"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -3144,7 +3158,7 @@
       <c r="L47" s="4"/>
       <c r="M47" s="4"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>119</v>
       </c>
@@ -3171,7 +3185,7 @@
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -3186,7 +3200,7 @@
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>121</v>
       </c>
@@ -3213,7 +3227,7 @@
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>121</v>
       </c>
@@ -3240,7 +3254,7 @@
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -3255,7 +3269,7 @@
       <c r="L52" s="4"/>
       <c r="M52" s="4"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>126</v>
       </c>
@@ -3280,7 +3294,7 @@
       <c r="L53" s="3"/>
       <c r="M53" s="3"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -3295,7 +3309,7 @@
       <c r="L54" s="3"/>
       <c r="M54" s="3"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>129</v>
       </c>
@@ -3320,7 +3334,7 @@
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -3335,7 +3349,7 @@
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>131</v>
       </c>
@@ -3362,7 +3376,7 @@
       <c r="L57" s="3"/>
       <c r="M57" s="3"/>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -3377,7 +3391,7 @@
       <c r="L58" s="3"/>
       <c r="M58" s="3"/>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>134</v>
       </c>
@@ -3404,7 +3418,7 @@
       <c r="L59" s="4"/>
       <c r="M59" s="4"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -3419,7 +3433,7 @@
       <c r="L60" s="4"/>
       <c r="M60" s="4"/>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>136</v>
       </c>
@@ -3446,7 +3460,7 @@
       <c r="L61" s="3"/>
       <c r="M61" s="3"/>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -3461,7 +3475,7 @@
       <c r="L62" s="3"/>
       <c r="M62" s="3"/>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>138</v>
       </c>
@@ -3488,7 +3502,7 @@
       <c r="L63" s="4"/>
       <c r="M63" s="4"/>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
@@ -3503,7 +3517,7 @@
       <c r="L64" s="4"/>
       <c r="M64" s="4"/>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>141</v>
       </c>
@@ -3530,7 +3544,7 @@
       <c r="L65" s="3"/>
       <c r="M65" s="3"/>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>141</v>
       </c>
@@ -3574,15 +3588,15 @@
       <selection pane="bottomLeft" activeCell="A3" sqref="A3:E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="22.44140625" customWidth="1"/>
+    <col min="1" max="2" width="22.42578125" customWidth="1"/>
     <col min="3" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="28.44140625" customWidth="1"/>
+    <col min="5" max="5" width="28.42578125" customWidth="1"/>
     <col min="6" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
         <v>25</v>
       </c>
@@ -3593,7 +3607,7 @@
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
     </row>
-    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -3616,7 +3630,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -3624,7 +3638,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -3635,7 +3649,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -3643,7 +3657,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -3654,7 +3668,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>70</v>
       </c>
@@ -3662,7 +3676,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>150</v>
       </c>
@@ -3673,7 +3687,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>151</v>
       </c>
@@ -3684,7 +3698,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>153</v>
       </c>
@@ -3695,7 +3709,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>155</v>
       </c>
@@ -3706,7 +3720,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>95</v>
       </c>
@@ -3714,7 +3728,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>157</v>
       </c>
@@ -3725,7 +3739,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>158</v>
       </c>
@@ -3736,7 +3750,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>159</v>
       </c>
@@ -3747,7 +3761,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>161</v>
       </c>
@@ -3758,7 +3772,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>105</v>
       </c>
@@ -3766,7 +3780,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>114</v>
       </c>
@@ -3774,7 +3788,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>164</v>
       </c>
@@ -3785,7 +3799,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>119</v>
       </c>
@@ -3793,7 +3807,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>121</v>
       </c>
@@ -3804,7 +3818,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>126</v>
       </c>
@@ -3815,7 +3829,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>129</v>
       </c>
@@ -3826,7 +3840,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>131</v>
       </c>
@@ -3834,7 +3848,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>134</v>
       </c>
@@ -3842,7 +3856,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>136</v>
       </c>
@@ -3850,7 +3864,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>138</v>
       </c>
@@ -3858,7 +3872,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>141</v>
       </c>
@@ -3880,13 +3894,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="29.44140625" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3894,7 +3908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>166</v>
       </c>
@@ -3902,7 +3916,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -3910,7 +3924,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -3918,7 +3932,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -3926,7 +3940,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>171</v>
       </c>
@@ -3934,12 +3948,12 @@
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -3947,7 +3961,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -3955,7 +3969,7 @@
         <v>45388.62510806237</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -3963,7 +3977,7 @@
         <v>45388.62510806237</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>

</xml_diff>